<commit_message>
Day 1 | Final Commit
</commit_message>
<xml_diff>
--- a/Batch/15/In_Class/Day_1.xlsx
+++ b/Batch/15/In_Class/Day_1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\In_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCD6AEE-C94E-4B71-AB84-8C7C72B930AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B7B61-D0A6-4A99-9E3E-2FB80E0D8602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" xr2:uid="{45576B8F-30EF-40A1-BD70-667D7EAAD699}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{45576B8F-30EF-40A1-BD70-667D7EAAD699}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
     <sheet name="Guideline" sheetId="2" r:id="rId2"/>
+    <sheet name="Intro TO Excel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="364">
   <si>
     <t>Name</t>
   </si>
@@ -2560,13 +2561,580 @@
       </rPr>
       <t>: Leveraging HR data to improve hiring practices, employee satisfaction, and organizational culture.</t>
     </r>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>ML Engineer</t>
+  </si>
+  <si>
+    <t>ETL Developer</t>
+  </si>
+  <si>
+    <t>Data Pipelines</t>
+  </si>
+  <si>
+    <t>Data Architect</t>
+  </si>
+  <si>
+    <t>Dashaboard</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain </t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Store Data in Tabular Format</t>
+  </si>
+  <si>
+    <t>Spread Sheet</t>
+  </si>
+  <si>
+    <t>Organise the data</t>
+  </si>
+  <si>
+    <t>Visualization</t>
+  </si>
+  <si>
+    <t>Format The Data</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Manage the Data</t>
+  </si>
+  <si>
+    <t>Analyse the data</t>
+  </si>
+  <si>
+    <t>TnA</t>
+  </si>
+  <si>
+    <t>Management of Task / Operations</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>4k</t>
+  </si>
+  <si>
+    <t>6k</t>
+  </si>
+  <si>
+    <t>Microsoft 365 - Personal</t>
+  </si>
+  <si>
+    <t>Microsoft 365 - Family</t>
+  </si>
+  <si>
+    <t>Microsoft Office 2021</t>
+  </si>
+  <si>
+    <t>Microsoft Online</t>
+  </si>
+  <si>
+    <t>WPS Office</t>
+  </si>
+  <si>
+    <t>Crack Version</t>
+  </si>
+  <si>
+    <t>File Extension For Excel</t>
+  </si>
+  <si>
+    <t>.xls</t>
+  </si>
+  <si>
+    <t>.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <t>XLS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XLSX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are both file formats for Microsoft Excel spreadsheets, but they have some key differences:</t>
+    </r>
+  </si>
+  <si>
+    <t>1. XLS</t>
+  </si>
+  <si>
+    <r>
+      <t>Format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLS is the older Excel file format, used by Microsoft Excel versions 97–2003.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>File Extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.xls</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: It uses a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>binary format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to store data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Compatibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLS files are compatible with older versions of Excel and some older third-party applications.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>File Size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLS files can be larger because of the binary format.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Limitations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Supports a maximum of 65,536 rows and 256 columns per worksheet.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. XLSX</t>
+  </si>
+  <si>
+    <r>
+      <t>Format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLSX is the newer Excel file format, introduced in Microsoft Excel 2007 and used by all newer versions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>File Extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: It uses an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Open XML format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, which is based on XML and ZIP compression.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Compatibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLSX files are not natively compatible with older Excel versions (Excel 2003 and earlier) unless a compatibility pack is installed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>File Size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XLSX files are generally smaller than XLS files due to ZIP compression.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Limitations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Supports a maximum of 1,048,576 rows and 16,384 columns per worksheet.</t>
+    </r>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>XLS</t>
+  </si>
+  <si>
+    <t>File Extension</t>
+  </si>
+  <si>
+    <t>Format Type</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Excel Version</t>
+  </si>
+  <si>
+    <t>Excel 97–2003</t>
+  </si>
+  <si>
+    <t>Compatibility</t>
+  </si>
+  <si>
+    <t>Older Excel versions</t>
+  </si>
+  <si>
+    <t>File Size</t>
+  </si>
+  <si>
+    <t>Generally larger</t>
+  </si>
+  <si>
+    <t>Row Limit</t>
+  </si>
+  <si>
+    <t>65,536 rows</t>
+  </si>
+  <si>
+    <t>Column Limit</t>
+  </si>
+  <si>
+    <t>256 columns</t>
+  </si>
+  <si>
+    <t>Which Format to Use?</t>
+  </si>
+  <si>
+    <r>
+      <t>XLSX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is recommended if you’re using modern versions of Excel and need larger datasets, as it offers better performance and smaller file sizes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>XLS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be useful if you need compatibility with older systems that don’t support XLSX files, although this format is largely outdated.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In general, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XLSX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the preferred format for its efficiency, support for larger data ranges, and compatibility with modern applications.</t>
+    </r>
+  </si>
+  <si>
+    <t>XLSX</t>
+  </si>
+  <si>
+    <t>Open XML (XML and ZIP)</t>
+  </si>
+  <si>
+    <t>Excel 2007 and newer</t>
+  </si>
+  <si>
+    <t>Newer Excel versions</t>
+  </si>
+  <si>
+    <t>Generally smaller</t>
+  </si>
+  <si>
+    <t>1,048,576 rows</t>
+  </si>
+  <si>
+    <t>16,384 columns</t>
+  </si>
+  <si>
+    <t>Components of the Excel</t>
+  </si>
+  <si>
+    <t>Menu / Tab</t>
+  </si>
+  <si>
+    <t>Ribbion</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Commands</t>
+  </si>
+  <si>
+    <t>Name Box</t>
+  </si>
+  <si>
+    <t>Formulae Bar</t>
+  </si>
+  <si>
+    <t>Siraj</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Horizontal Space</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Vertical Space</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Alphabets</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Cell Address</t>
+  </si>
+  <si>
+    <t>D113</t>
+  </si>
+  <si>
+    <t>Search Box</t>
+  </si>
+  <si>
+    <t>Sheets</t>
+  </si>
+  <si>
+    <t>Scroll Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Layout </t>
+  </si>
+  <si>
+    <t>Customize Quick Access Bar</t>
+  </si>
+  <si>
+    <t>Customize a Ribbion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2598,8 +3166,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2609,6 +3182,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2625,20 +3210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2650,6 +3226,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2722,6 +3321,1477 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>522775</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>19351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E550F93-5BB4-4FE0-B530-A41F27DFB1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2167759" y="11771586"/>
+          <a:ext cx="7577844" cy="382451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>58241</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>141967</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E8DA6ED-6623-4AB1-B54B-1146A6C24B02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2167759" y="12691241"/>
+          <a:ext cx="18168879" cy="1066386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107673</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>57978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>411881</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16988</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A screenshot of a computer&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDB7303-C9A5-466D-8F8D-676D930AF3ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2277716" y="14105282"/>
+          <a:ext cx="1695687" cy="1052315"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381053</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>96172</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C986C6E-12A4-4A62-BE6F-361969354BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2171700" y="15573375"/>
+          <a:ext cx="381053" cy="272385"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47720</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>125631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50AB6EE6-EB41-409A-B516-B985D122330A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2914650" y="15592425"/>
+          <a:ext cx="695420" cy="287556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1266986</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>173264</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB625D8C-C42E-4599-902F-081FB05C2EDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2266950" y="16325850"/>
+          <a:ext cx="1171736" cy="325664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>383348</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>75176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F572F93B-0509-48B4-BC7F-8F37CA38A617}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2171700" y="17202150"/>
+          <a:ext cx="17147348" cy="432364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1834243</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>92528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314711</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>75985</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F40D3C0-A7D8-49B0-B8DC-8597FB564705}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2051957" y="18609128"/>
+          <a:ext cx="11369835" cy="701914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>283029</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>550961</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>742</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB3F11FD-3E81-D07D-C735-6EDE9BC7DE66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2454729" y="20938672"/>
+          <a:ext cx="3958189" cy="452499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175477</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>166409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>122747</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>94207</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B5C193-D278-1A4F-B971-436FFBD7D36A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8105040" y="20716597"/>
+            <a:ext cx="596160" cy="999360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B5C193-D278-1A4F-B971-436FFBD7D36A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8098887" y="20710640"/>
+              <a:ext cx="608467" cy="1011274"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352237</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>108089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>362759</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>133371</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EA5598B-FC95-CF81-506C-99920164494D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8281800" y="20658277"/>
+            <a:ext cx="5760" cy="20520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EA5598B-FC95-CF81-506C-99920164494D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8275680" y="20652157"/>
+              <a:ext cx="18000" cy="32760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>380399</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>135498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2147</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>122144</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D698E4E-9F34-94B9-498E-7C62E661444D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8309962" y="20864279"/>
+            <a:ext cx="270638" cy="165240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D698E4E-9F34-94B9-498E-7C62E661444D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8303836" y="20858146"/>
+              <a:ext cx="282891" cy="177507"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>221027</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>41782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>445389</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>8072</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D570C118-FD1B-98CB-2B0F-28335C8910AD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8799480" y="20949157"/>
+            <a:ext cx="219600" cy="135360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D570C118-FD1B-98CB-2B0F-28335C8910AD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8793360" y="20943037"/>
+              <a:ext cx="231840" cy="147600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>620709</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>162138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390940</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>134628</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="28" name="Ink 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ABC181E-3ADE-D167-3057-0E4BDB2056CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9199162" y="20890919"/>
+            <a:ext cx="414360" cy="329678"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="28" name="Ink 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ABC181E-3ADE-D167-3057-0E4BDB2056CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9193042" y="20884801"/>
+              <a:ext cx="426600" cy="341915"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>637016</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>2264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>610370</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>9152</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="36" name="Ink 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{181F26E4-35E3-4100-CC49-0EF593683759}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9864360" y="20909639"/>
+            <a:ext cx="617482" cy="180720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="36" name="Ink 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{181F26E4-35E3-4100-CC49-0EF593683759}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9858239" y="20903519"/>
+              <a:ext cx="629724" cy="192960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>376357</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>83283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>535477</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>85016</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="37" name="Ink 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D909CE7-E9B9-176C-4E01-2844D793FDC0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8305920" y="20454877"/>
+            <a:ext cx="159120" cy="358920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="37" name="Ink 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D909CE7-E9B9-176C-4E01-2844D793FDC0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8299800" y="20448757"/>
+              <a:ext cx="171360" cy="371160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>274559</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>57513</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400408</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>46693</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="67" name="Ink 66">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54EC62A-B2E7-2AA8-8A37-9CC8D07B433F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8204122" y="20071919"/>
+            <a:ext cx="2072520" cy="524962"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="67" name="Ink 66">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54EC62A-B2E7-2AA8-8A37-9CC8D07B433F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8197966" y="20065958"/>
+              <a:ext cx="2084833" cy="536885"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352338</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>67030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>236690</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>45689</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="72" name="Ink 71">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39429DE-6186-3D9C-7832-6DCB57F4A671}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9579682" y="21152999"/>
+            <a:ext cx="528480" cy="514440"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="72" name="Ink 71">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39429DE-6186-3D9C-7832-6DCB57F4A671}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9573636" y="21147066"/>
+              <a:ext cx="540572" cy="526306"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>474991</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>40323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>113639</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>46783</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="97" name="Ink 96">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF96665-1D74-EEE7-055B-9DE24B05F7B8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2647882" y="21483479"/>
+            <a:ext cx="5395320" cy="537480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="97" name="Ink 96">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF96665-1D74-EEE7-055B-9DE24B05F7B8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2641760" y="21477588"/>
+              <a:ext cx="5407565" cy="549262"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542494</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>170517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="Picture 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CED1CE0B-6413-4230-A339-74676F0E634B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2172891" y="22514719"/>
+          <a:ext cx="6948056" cy="349111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>65484</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1030216</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>106222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="Picture 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985CD924-B200-4E1C-A8D5-1C54B079223B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2238375" y="23348157"/>
+          <a:ext cx="2353001" cy="339584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:13:47.841"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 27178,'0'2851'0,"1646"-2851"0,-1646-2851 0,-1646 2851 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:15:54.591"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 556 12566,'0'0'9513,"1"-16"-7077,2 26-2438,-1 1 0,0-1 0,0 1 0,-1 0 0,0 13-1,2 22 51,14 55 63,5 179-1,-22-280 277,0-7-205,0-2-205,1 1 0,0 0 0,0 0 0,1 0 0,0 0 1,0 0-1,1 0 0,0 0 0,0 1 0,1-1 0,0 1 1,5-7-1,8-9-100,0 1 0,26-24 0,-28 32 57,-1 0 0,-1-2 0,-1 1 0,0-2 0,18-31 0,-28 41 91,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0 0,0 0 0,-4-9 0,5 15-19,0 1-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0-1 0,-1 1 0,1 0 1,0 0-1,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,0 0 1,0 0-1,0 1 0,-1 23 60,1-22-88,0 221 247,2-209-229,1 1 1,0-1-1,0 0 0,1 0 1,1 0-1,0-1 0,14 24 1,-18-35-132,0 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 1 1,0-2-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 0,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,2-3 1,1 0-173,-1-1 0,1 1 0,-1-1 1,0 0-1,0-1 0,0 1 0,-1 0 0,0-1 1,0 0-1,0 0 0,-1 0 0,3-11 1,-2 1 998,-2 0 0,0-33 0,-1 32 4321,1 19-4955,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,0 4 1,0-2 25,-8 149 951,9-152-1031,0-1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,1 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,1 0 1,-1 0 0,0 0 0,0 1-1,1-1 1,-1-1 0,0 1 0,0 0-1,0 0 1,0 0 0,3-1 0,-1 0 8,1 0 1,0 0 0,-1-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0-1 1,-1 1 0,5-6-1,-4 4 5,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,-1 1 1,-1-5-1,2 6-8,-1-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,-4 0 0,8 0-17,0 0 0,0 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,15-9-249,29-11-45,-36 16 286,0-1 1,0 2-1,0-1 1,0 1-1,1 0 1,0 1-1,-1 0 1,1 1-1,0 0 1,0 0-1,10 1 1,-16 1 24,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,1 3-1,22 52 245,-14-32-124,-7-19-97,-3-4-25,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,3 1 0,-4-2-3,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1-1 0,12-38 142,-11 36-137,-1 1 11,1 1 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,1-2 0,-1 4-20,0 0-1,-1 0 1,1 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,2 3 1,2 0 4,1-1 1,0 0-1,0 0 0,0 0 0,0-1 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 0 0,1-1 1,-1 1-1,9-2 0,-12 2 1,0-1 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1-1 1,-1 1-1,0-1 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 1,0 0-1,0 0 0,0 1 1,1-7-1,-1 3 14,0-1 0,-1 1 0,0-1-1,0 0 1,0 1 0,-1-1 0,0 0 0,0 1-1,-1-1 1,0 1 0,0 0 0,0 0 0,-1 0-1,-6-11 1,6 13 8,0-1 0,-1 2-1,0-1 1,0 0 0,0 1 0,0 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,0 1 0,0 0 0,0 0-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,-6 1 0,7 0-27,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1-1,-1-1 1,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,-4 2 0,4-1-55,1-1-1,0 0 0,0 1 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1-1-1,0 1 0,-1 0 0,2 0 1,-1 0-1,0 0 0,0 1 1,1-1-1,0 0 0,0 4 1,-1-3-153,0 55-2794,10-22-4324,12-8-4501</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1823.72">1221 829 10197,'0'0'9449,"0"0"-9381,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,1-1-1,-1 1 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,0 1 1,0-1 0,0 0-1,1 0 1,-1 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 1-1,5 18 119,-1 0-1,-1 0 0,-1 1 1,-1-1-1,-1 22 1,0-41-26,11-32 504,-10 28-659,3-8-27,0 1 0,0-1 0,2 1 0,7-13 0,-13 23 18,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,2-1 0,-2 2 2,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 1 0,1-1 0,1 3 0,12 23 35,15 26 70,-28-53-101,-1 1-1,1 0 1,-1-1-1,1 1 1,-1-1-1,1 0 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,-1-1 1,1 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 0 1,17-24 41,-16 21-20,54-78 14,-55 81 3,9 33-21,-10-32-22,3 16 109,1 0 1,1 0-1,1-1 1,7 15-1,-12-26-184,1-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1-1-1,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,0-1 0,0 1 1,0 0-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 1,1-1-1,-1 1 1,7 0-1,-6-1-112,0-1-1,0 1 1,-1-1-1,1 1 1,0-1 0,0 0-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1 0,-1 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,0 0 1,-1-1 0,4-7-1,-2 2 368,0-1-1,-1 1 1,0-1-1,-1 0 1,0 0-1,0 0 1,-1 0-1,0 0 1,0 0-1,-3-13 1,3 22-112,-1 0 0,1-1 0,0 1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 1,0-1-1,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,0 0 0,0 2 0,-4 8-36,1 1 0,0 0 0,1 0-1,0 0 1,1 1 0,0-1 0,1 0-1,0 1 1,2 19 0,-1-32-32,0 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0-1-1,0 1 1,1 0 0,-1-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 0 0,1 1-1,0-1 1,0 1 0,26-2-268,-22 0 222,0 0 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,8-5 0,-7 1 38,0 1 1,0-1-1,-1 0 1,0 0-1,0 0 0,0-1 1,-1 1-1,0-1 1,-1 0-1,0 0 1,2-13-1,-4 21 695,11 29-795,-9-25 111,0 0 0,0-1-1,1 1 1,-1 0 0,1-1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0-1 0,0 0-1,0 1 1,0-1 0,0-1 0,1 1 0,-1-1-1,0 0 1,0 0 0,1 0 0,-1 0 0,8-3-1,-10 3 3,-1-1-1,1 0 1,0 0-1,-1 0 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0-3 1,9-23 197,-9 27-16,0 24-359,0-21 180,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,1 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,1 0-1,-1 1 0,0-1 1,2 1-1,0-2-11,-1 0-1,0 0 1,0 0 0,0 0 0,1-1 0,-1 1-1,0 0 1,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,0 0 0,-1 1-1,3-3 1,6-5-65,-3 2 39,0 1-1,0-1 1,-1 0 0,0-1 0,7-10 0,13 77 101,-25-56-78,0 0-1,1 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 0 0,0 1 1,0-1-1,0-1 0,0 1 0,0 0 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 0 1,3-4-1,-1 2-65,0 0 1,-1-1 0,0 0-1,0 0 1,-1 0 0,1-1-1,-1 1 1,0-1 0,-1 0-1,1 0 1,-1 0-1,3-11 1,-2-1 298,-1 0-1,-1 0 1,-1-23 0,0 36-72,-14 58 100,8 358-171,7-266-4,-2-135-66,1-1 0,-1 1 1,-1-1-1,0 0 0,0 1 1,0-1-1,-1 0 1,-1 0-1,0-1 0,0 1 1,0-1-1,-1 0 1,-7 9-1,9-12 27,-1-1 1,1 0-1,-1 0 0,0 0 1,-1 0-1,1-1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0-1-1,0 0 0,0 0 1,-1 0-1,1-1 1,0 0-1,-1 0 0,1 0 1,-1-1-1,1 0 0,-1 0 1,1 0-1,-10-2 0,11 0-16,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,0-1 0,0 1 0,-1-1 0,2 0 0,-1 0 0,0 0 0,-1-7 0,-3-6-19,1-1 1,1 1 0,-3-31 0,3 8-150,1 0 1,4-61 0,0 87-116,0-1-1,2 1 1,0-1-1,0 1 1,1 0-1,1 0 1,0 1-1,1-1 1,1 1-1,10-17 1,32-39-7756,-26 40-1776</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4068.26">2742 928 5491,'0'0'17023,"3"-15"-16652,3-17 239,-1 1 0,0-47 0,-6 60-464,0-17 367,5 29-379,6 14-241,10 17 98,2-1 0,1-1 0,33 26 0,-36-32-4,1 0 0,-2 1 0,0 2 0,-2 0-1,31 43 1,-46-59-7,0 1-1,0-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,0 0 0,0 0 0,0-1 1,0 1-1,-2 9 0,1-12 25,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,-2-2 0,3 1 8,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 1,0-3-1,0-41-21,1 30 20,1 1-25,0 0 1,1 0-1,1 0 1,0 1-1,1-1 1,1 1-1,0 0 1,0 1-1,1-1 1,10-13-1,22-46-144,-32 57 151,-2 0 1,0-1-1,-1 0 0,-1 0 0,0 0 1,-1-1-1,0 1 0,-2-1 1,0-19-1,-2 25 84,-3 13-25,-2 19-77,4 18 64,1-1 0,2 1-1,2-1 1,1 0 0,16 76-1,-17-107-33,0 1-1,0-1 1,0 0 0,1 0-1,0 0 1,1 0-1,7 12 1,-10-18-8,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,2-3 1,31-23-66,-30 22 45,-1 1 0,1 0-1,0 0 1,0 0 0,0 1 0,0 0 0,1 0-1,-1 1 1,1-1 0,0 1 0,0 0 0,0 1-1,0-1 1,0 1 0,8 0 0,-13 1 22,0 1-1,0-1 1,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 2 1,11 29 48,-8-23-8,6 27 130,-6-26-84,-1 0 0,1 0 0,0-1 1,8 16-1,-10-22-74,1-1-1,-1 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1-1,0-1 1,0 1 0,0-1-1,1 1 1,-1-1-1,0 0 1,0 0 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1 0,1 0-1,-1 1 1,4-1-1,0-1-3,-1 1-1,1-1 1,0 0-1,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1-1-1,-1 0 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1-1-1,-1 1 1,5-6-1,-3 2-7,0 1 0,-1-1-1,0 1 1,0-1 0,0 0 0,-1-1-1,0 1 1,-1-1 0,0 1-1,0-1 1,-1 0 0,1-12-1,-2 12 2,1-2-15,-1 0 0,-1 0 1,0 0-1,-4-17 0,5 27 14,0-1-1,-1 1 1,1 0 0,0 0 0,-1 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,-2 0 1,2 0 1,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 1,-1 0-1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 2 0,-3 0 1,2 1 1,-1 0-1,0 1 1,1-1-1,0 1 1,0-1-1,0 1 1,0 0-1,1 0 1,0 0 0,0 0-1,0 1 1,1-1-1,-2 10 1,0 6 1,1 0 1,1 31 0,1-50-3,0 0-2,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1 0,0-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 0 0,1 1-1,1 0 3,0-1-1,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 0 0,8 0 0,-1-1 2,-1 0 0,1-1 0,-1 0-1,1-1 1,-1 0 0,0-1 0,10-5 0,-11 4-19,0-1 1,-1 0-1,0 0 1,1-1 0,-2 0-1,1 0 1,-1-1-1,8-11 1,-11 13 5,0 0 0,-1-1 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1-9 0,0 15 8,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 1 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,-1 1-1,-1 3 1,0 1-1,0 0 0,0 0 1,0 0-1,1 1 0,0-1 1,0 0-1,1 1 0,0 0 1,0-1-1,0 10 0,0 6-2,1-1 0,3 29-1,-3-47 6,1 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,1-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,1 1-1,-1 0 1,1-1 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,0 1-1,1-1 1,-1-1 0,4 2 0,-2-1 0,0 0 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,7-5 0,0-3 11,-1 0 0,0-1 1,-1 0-1,0 0 1,0-1-1,-1 0 1,-1-1-1,0 0 1,-1 0-1,8-28 0,-7 12-9,-1 0-1,-2-1 1,-1 1-1,-1-47 1,-2-64 74,-2 193-95,1 112 171,3-143-132,0 1 1,1-1-1,0 0 1,2-1 0,1 1-1,10 25 1,-11-35-17,0 0 0,1 0 0,1-1 0,0 1 0,0-2 0,15 17 0,-19-24-6,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,4-3 0,-4 1 5,1-1 0,-1 0 1,0 0-1,-1 0 1,1-1-1,-1 1 0,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,0 0 0,0-1 1,2-10-1,2-7 16,-1 0 0,2-29 0,-4 16-6,-1 0 1,-6-61-1,4 96-13,0 1-1,0-1 1,1 0 0,-1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 0 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 1-1,1-1 1,-1 1 0,0 0 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0 0,1 1 1,0-1-1,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,-1 2-1,-2 14 2,0-1 1,2 1-1,0 0 1,0 1-1,2-1 1,0 0 0,5 23-1,-3-31-5,-1 0 0,2-1 0,0 1 1,0-1-1,0 1 0,1-1 0,1-1 0,-1 1 0,1-1 0,1 0 0,-1 0 0,1-1 1,1 0-1,9 8 0,22 20 29,-38-35-54,-28 0-1182,-12-5-1835,11-3-2054,-15-8-5448</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4241.61">3818 798 11477,'0'0'9445,"107"-35"-9445,-63 23-1409,-15 1-2689,-9 5-8228</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5020.26">4847 764 9877,'0'0'12098,"-1"0"-12051,1-1 0,-1 1-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,0 0-1,-1 2 1,0 29 441,0-12-263,0-1 0,5 33 1,-4-48-215,0 1 1,1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,1-1 0,-1 1-1,1-1 1,0 0 0,0 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,1 1 0,0 0-1,5 3 1,-7-5-14,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,3-3 0,27-48 187,-20 31-138,-10 21-50,0-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,0 0 0,1 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1 0,-1 1-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,1 0 1,10 23-141,-9-15 169,0 1-19,1 0 0,0-1 0,1 1 1,-1-1-1,1 0 0,10 12 0,-12-17 2,0 0-1,0-1 1,0 1-1,1-1 1,-1 1-1,1-1 1,-1 0-1,1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 0 1,5 1 0,-8-2-3,0 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,1 0 0,-1 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0-1-1,0-29 75,0 24-39,1-18 124,-1 18-189,1 1 1,-1-1-1,0 0 1,0 0-1,-1 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,-3-8-1,4 12-507</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5295.79">5173 871 8148,'0'0'10332,"12"-2"-8958,-6 2-1220,1-1 0,0-1 0,-1 1-1,1-1 1,-1 0 0,0-1 0,1 0-1,-1 0 1,-1 0 0,1-1 0,0 0-1,-1 0 1,1 0 0,-1-1 0,0 1 0,-1-2-1,1 1 1,5-9 0,-7 10-26,0 1 1,-1-1 0,0 0 0,1 0-1,-1 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,0-1 0,0 1-1,0-1 1,-1 0 0,0 1 0,0-8-1,-2 12-73,-1 0 0,0 0-1,1 1 1,-1-1 0,0 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-4 2 0,0 5-48,-1-1 1,1 1 0,1 0 0,0 0-1,0 1 1,0-1 0,1 1-1,0 0 1,1 1 0,-1-1 0,2 1-1,0-1 1,0 1 0,0 0 0,1 0-1,1 0 1,-1 0 0,3 14-1,-2-22-49,1 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,1 1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,0-1 0,-1 0 0,1 1-1,0-1 1,0 0 0,4 1-1,0 1-693,1-1-1,0 0 1,0 0 0,1 0-1,12 0 1,23-1-5024</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5590.88">5692 835 12982,'0'0'10183,"-14"4"-8897,11-1-1191,0 0-1,1 1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 1-1,0-1 0,0 1 1,0 8-1,-3 62 237,4-73-343,0 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,2 1 0,7 1-416,1-1 0,-1 0 0,19-1 0,-15-1-327,2 0-613,1-1 1,-1-1-1,1-1 0,-1 0 0,0-2 0,-1 0 1,1-1-1,-1 0 0,28-19 0,-4 3-5038</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6279.57">6051 841 5555,'0'0'14478,"-10"-10"-13192,-30-31-507,39 41-757,0-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1-1,0-1 1,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1-1,-1 0 1,-14 22 221,13-18-134,-2 4-15,0 0 1,0 1 0,1-1 0,0 1 0,0 0-1,1 1 1,1-1 0,-1 0 0,2 1 0,-1-1 0,2 1-1,-1 17 1,2-27-102,-1 0-1,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,0-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,0 0 0,37-10-450,-32 7 382,0-1 1,0 0 0,-1 0-1,0 0 1,0-1 0,0 0-1,0 0 1,-1 0 0,0 0-1,0-1 1,-1 0 0,0 1-1,0-2 1,0 1 0,-1 0-1,3-12 1,-2 61 2295,-3-39-2222,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,4 2 0,-2-2-57,1 0 1,0-1-1,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 0,1 0 1,-1-1-1,0 1 0,0-1 1,6-4-1,-2-1-45,1 0 0,-1 0 0,-1-1 0,1 0 0,-1 0-1,10-18 1,-13 92 2007,-4-65-1908,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0 0 1,1-1-1,13-11-97,32-67-341,-46 79 473,1 1 0,-1-1 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,0 1 1,0-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1-1,0 0 1,0 0 0,8 33 193,-6-26-53,-1-4-217,-1 2-47,1-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,4 4 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7699.51">6982 853 15575,'0'0'8671,"-11"-11"-8082,-36-29-215,45 38-353,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 1 1,0-1 0,1 1-1,-1-1 1,-1 3 0,-1 2-23,0 0-1,0 0 1,1 1 0,0-1 0,0 1 0,0 0-1,-2 11 1,2-5-20,1-1-1,0 1 0,1-1 1,0 1-1,1 0 0,0 0 0,2 12 1,-1-24 5,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,1 0 0,30-16-211,-23 7 191,0-1-1,0 1 0,-1-1 0,0-1 1,-1 0-1,10-22 0,-15 40 105,0 0 0,1 0-1,-1 0 1,1 0 0,1 0-1,-1 0 1,1-1 0,-1 0 0,2 0-1,-1 0 1,7 6 0,-7-9-296,-1 0 0,1 0 0,0-1 0,0 0 1,0 1-1,1-2 0,-1 1 0,0 0 0,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 1,0 0-1,-1-1 0,6-3 0,-5 2 102,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,0-1 1,0 1-1,0 0 1,-1-1 0,1 1-1,-1-1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0-11 1,-1 16 223,0 1 0,1-1 1,-1 0-1,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 1 0,0-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 1 0,-1-1 1,0 0-1,1 0 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 1 0,1-1 1,-1 1-1,-3 1-13,1 0 0,0 0-1,1 1 1,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-4 6 0,3-2-51,1 1 0,-1 0 0,1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,1 1 0,1 11 0,-1-14-28,0-5-7,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,0 0 0,-1-1 0,1 1 0,0 0-1,-1-1 1,1 1 0,0-1 0,0 1 0,0-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,2-1 0,1 1-17,0-1 1,-1 1-1,1-1 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 0 1,5-1-1,0-3-65,-1-1-1,0 0 0,0 0 1,0 0-1,-1-1 1,0 0-1,0 0 0,-1 0 1,0-1-1,0 0 0,-1 0 1,0-1-1,-1 1 1,0-1-1,3-14 0,0-11 155,-2 0-1,-2 0 0,-2-40 1,0 53 272,0 22 35,0 3-320,0 36 31,-1-12-30,1-1 1,1 1-1,1-1 1,9 42 0,-9-61-56,0 0 0,0 0 0,0 0 0,1-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,1-1 1,-1 1-1,1-1 0,0 0 0,-1 0 0,2-1 0,-1 0 0,0 0 0,9 2 0,-9-3-8,0 0 1,0 0-1,0-1 1,0 0-1,0 0 1,0-1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 0-1,10-3 1,-13 3 4,0-1 0,0 1 1,1-1-1,-1 0 0,-1 0 1,1-1-1,0 1 0,0 0 1,-1-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0-1 1,-1 1-1,1 0 0,-1 0 1,0-1-1,0 1 0,0-1 1,1-6-1,0 1 18,-1 1-1,0-1 1,0 1-1,-1-1 1,0 1 0,-1-1-1,1 0 1,-2 1 0,-1-9-1,2 14 8,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,1 1-1,-1 0 1,-5 0 0,5 0-5,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1 1 1,0-1-1,0 1 0,-3 5 1,2-1-24,0 0 1,1 0 0,0 0 0,0 0 0,0 1 0,1-1-1,0 1 1,1-1 0,0 13 0,0-19-3,0 0 1,1 0 0,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1-1,0 1 1,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 1-1,0-1 1,0 0-1,0 1 1,0-1 0,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,3 1 2,-1 0-1,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 0 1,0-1-1,4-1 0,1-4 0,-1 0 0,0 0 1,0-1-1,-1 0 0,0 0 0,0-1 0,6-12 0,30-72-20,-36 72 30,-1-1 0,-2 1-1,0-1 1,-1 0 0,-1 0 0,-1 0-1,0 0 1,-6-28 0,4 39 4,-1 12-72,-1 19-11,0 74 102,0-48 53,4 49-1,0-83-79,1 1-1,1-1 0,0 0 0,1 1 1,0-1-1,1 0 0,0-1 1,10 20-1,-10-23-574,10 18 1060,-3-17-8356</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8728.66">7974 858 14038,'0'0'6289,"25"6"-4699,-22-6-1531,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,0-1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0-2-1,2-9-16,0-1 0,-1 1-1,-1 0 1,-1-25-1,0 31 62,0 7-11,0 42-58,0-32-33,0-1 0,1 1 1,0 0-1,0-1 0,1 1 0,0-1 1,4 11-1,-5-16-2,0 0 0,1-1 0,-1 1 0,1 0-1,0-1 1,-1 0 0,1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,5-1 0,-2 1-21,0 0 1,0-1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,0-1 1,-1 1 0,1-1-1,0-1 1,-1 1 0,1-1-1,-1 0 1,0 0 0,0 0-1,0-1 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1-1,0 0 1,-1 0 0,7-10 0,-10 15 35,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 1,1-1-1,0 30-114,-1-22 180,2 23 41,-1-5-15,1 0 0,0 0 1,2-1-1,10 34 1,-14-56-98,0 0 1,1-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,-1 0-1,1-1 0,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 1,0 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 1,1 0-1,-1-1-1,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,-1-1 1,0 1 0,3-2 0,5-8 15,0-1 0,0 0-1,-1 0 1,7-14 0,-13 23-23,22-44-98,29-77-1,-53 123 92,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1-1,0 1 1,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1-1,1 1 1,1 0 0,33 29-17,-27-21 38,-4-6-6,1 1 1,-1-1 0,1 1-1,0-1 1,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1-1-1,1 0 1,-1 0 0,1 0 0,0-1-1,7 0 1,-12 0-93,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,0-1 0,1-24-5844,-2 20 2632,1-14-7974</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8873.86">8164 486 13094,'0'0'7700,"29"-3"-9365,-14 3-3089</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10116.94">9124 700 12134,'0'0'7787,"-3"7"-7389,-3 14 29,0-1 1,2 1 0,0 0-1,1 0 1,1 0-1,1 34 1,2-54-416,-1-1 0,0 1 0,1 0 0,0 0 1,-1-1-1,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,30-3 240,-29 2-233,0 0 1,0 0-1,0-1 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 1,2-7-1,-1 4 3,0 0 1,-1-1-1,0 1 0,0-1 1,-1 1-1,0 0 0,0-1 1,-2-10-1,1 17-19,1-1 1,-1 1-1,0-1 1,1 1-1,-1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-3 1-1,2-1-10,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0-1,-1 2 1,1-3-7,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 1,-1-1-1,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 1,-1-1-1,1 0 0,0 1 0,1-1 0,32 2-202,38-21-35,-67 17 207,6-1-5,0 0-1,0 0 0,0 1 0,0 0 0,12 0 1,-20 4 52,-1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 1 1,1-1-1,-1 1 1,1-1 0,-1 1-1,0 0 1,0-1-1,0 1 1,0 0 0,0 0-1,0 4 1,4 7 44,24 55 197,-29-68-231,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 1 0,2-2 0,28-23 164,-20 14-186,32-31 68,-40 41-62,0-1-1,-1 1 1,1-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,3 1-1,-2 2 36,0 1-1,0 0 1,0 0-1,0 0 1,-1 1-1,0-1 1,1 1-1,-2-1 1,1 1-1,0 0 1,1 9-1,2 2 171,-3-11-150,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,0-1 0,0 0 0,0 0 0,9 6 0,-11-9-40,1 1 0,-1-1 0,0 0 0,1 0-1,-1-1 1,1 1 0,0 0 0,-1-1 0,1 0 0,-1 0-1,1 1 1,0-2 0,-1 1 0,1 0 0,0 0 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0-1,1-2 1,8-6 19,-1-2 0,-1 1-1,0-1 1,0-1 0,10-20-1,-16 28-39,-1-1 0,1 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,-1 0 1,-1 0 0,1-1-1,-1 1 1,0 0 0,0 0-1,-1-1 1,0 1 0,-2-9-1,2 14 6,1-1 1,-1 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 2 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 1 1,1-1-1,0 1 0,-2 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 1 1,1 0-1,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 1 1,-3 4-1,2 3-2,-1 1 1,1-1 0,1 1-1,0 0 1,1 0 0,-1-1-1,2 1 1,0 0 0,0 0-1,2 11 1,-2-20-5,1 0 0,-1 0 1,0 0-1,1 0 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 0 1,-1 0-1,3 2 0,0-1-108,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 0-1,7 1 1,8-1-2159,-1-1-1,36-5 1,-50 4 1430,44-8-6494</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10473.06">10283 477 11861,'0'0'9949,"1"9"-9543,3 70 835,-4-47-676,2 1-1,0-1 1,14 60 0,-15-89-552,0-1 0,0 1 0,0 0 1,0 0-1,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,3 0 0,-4 0-165,0 0 1,1-1-1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,1-1 0,-1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1-1 0,0 1 0,0-5 0,-3-28-8292,-9 20 2847</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10629.99">10283 685 7523,'0'0'14551,"-44"0"-14023,44-3-496,20-3 112,-1-3-96,11-2 16,4-1-64,-5 4-592,-5-4-672,-4 0-1810,-6 7-832,-9-7-3489</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10814.27">10259 450 12950,'0'0'6947,"58"-40"-6947,-33 40-16,-1 3-704,0 17-1601,-4 6-1377,-1-3-5042</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11209.7">10577 544 13494,'0'0'11171,"-5"10"-10833,-116 250 161,121-260-569,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,-3-13-1858,2-20 447,1 20 1370,3-54-198,8 27 2986,-10 39-2592,-1 1-1,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 0,1 1 1,-1 0-1,0-1 0,1 1 1,-1 0-1,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,18 28-398,-15-22 695,17 33-192,-14-26-351,1 1-1,0-2 0,0 1 1,12 13-1,-18-26-271,0 1-1,-1-1 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,0-1 1,1 1 0,-1-1-1,3 0 1,10 1-5921</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12036.67">10772 589 10053,'0'0'11231,"-1"19"-9734,-5 4-796,0-2-321,1 0 1,1 1 0,-2 21 0,6-39-358,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,0 0 0,0-1 1,0 1-1,0-1 0,1 0 1,-1 1-1,1-1 1,0 0-1,4 3 0,-2-3-12,0 0 0,1-1 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0-1-1,-1-1 1,1 1 0,0-1-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1-1 1,1-1 0,0 1 0,-1-1-1,1 0 1,-1-1 0,0 1 0,8-5-1,2-2 1,0-1-1,-1 0 1,0-1-1,-1 0 1,0-1-1,15-18 1,-25 26-29,1-1 1,-1 1 0,-1-1 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,2-10 0,-4 14 11,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 1 1,-1-1-1,-1 0 1,1 1-1,0-1 1,0 0-1,0 1 0,0 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,-1 1 1,-1-2-6,1 1 0,-1 1-1,0-1 1,1 1 0,-1-1 0,1 1-1,-1 0 1,0 0 0,1 1 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,-3 3 0,3-2 8,0 1 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,1 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,0 5-1,-1 2 34,1-6-18,0-1 0,1 0 0,0 0 1,0 1-1,0-1 0,2 12 1,-1-16-14,-1-1 1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1-1 0,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 0 0,0 1 0,0-1-1,-1 0 1,4 0 0,8 0-2,1 0-1,-1-1 0,0-1 0,0 0 1,0 0-1,0-1 0,0-1 1,-1-1-1,1 0 0,-1 0 1,0-1-1,-1-1 0,1 0 0,-1 0 1,0-2-1,-1 1 0,0-1 1,-1-1-1,1 0 0,-2 0 1,9-12-1,-9 10 3,0-1 0,-1 1 0,-1-2 1,0 1-1,0-1 0,-1 0 0,-1 0 0,0 0 0,2-19 1,-2-12-93,0-76 0,-4 107 58,-7-19 97,-1 26 70,-2 22-121,-3 18-2,3 1 0,0 1 0,2 0 0,2 0 0,1 0 0,1 1 0,2 0 0,3 44 0,0-66 30,1-1 1,0 1-1,1-1 1,1 1-1,0-1 1,1 0 0,0-1-1,1 1 1,8 13-1,-12-21-47,1 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 1,0 0-1,0 0 0,0 0 0,0-1 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0-1 0,9 0 0,-12 0-99,0-1 0,1 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1 0 0,1-1-1,0 0 1,-1 1-1,2-4 1,12-18-4637,-5 0-5215</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13137.31">11912 501 4418,'0'0'15925,"0"-7"-14575,0-20-297,0 20-1,0 10-882,0 47 46,9 68 0,-7-102-187,1 0 1,0 0-1,2 0 0,-1-1 0,2 1 0,0-1 0,1-1 0,11 20 0,-17-31-26,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,1 0 0,-1 0 0,0 1 0,1-2 0,-1 1 1,1 0-1,-1 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 1,-1-1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 1,0 1-1,1-3 0,19-63 183,-21 67-191,0 1-1,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0 0 1,0-1-13,9 13 13,-1-1 1,2 0 0,0 0-1,0-1 1,1-1 0,19 15-1,-24-21 11,0 0 0,1 0 0,-1-1 0,1 0 0,-1-1 0,1 1-1,0-1 1,0-1 0,0 1 0,0-1 0,0-1 0,0 1 0,0-1-1,0 0 1,0-1 0,9-2 0,-12 2-1,-1 0 1,0-1-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,-1-1 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,0-1 1,0 0-1,0-4 0,3-10 40,-2-1-1,0 1 1,-1-26-1,0 34-30,-1 0-1,0-1 1,-1 1-1,0 0 1,-1 0-1,0 0 0,0 0 1,-1 0-1,0 0 1,-1 1-1,0 0 1,-1-1-1,1 1 1,-2 1-1,1-1 1,-1 1-1,0 0 1,-14-13-1,19 20-44,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,1 0 0,-1 0 0,-1 2 0,0 2-590,-1-1-1,1 2 1,0-1 0,0 0-1,0 0 1,1 1 0,-2 9-1,-2 17-4807</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13850.74">12508 660 4434,'0'0'13521,"0"18"-12737,0 116 1134,0-133-1899,0 1-1,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 1,0 0-1,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0-1 0,2 1 0,1-1 15,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 0-1,0-1 1,1 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,4-5-1,-2 1 55,-1 0-1,0 0 1,-1-1-1,1 1 1,-1-1-1,0 0 0,-1 0 1,0 0-1,3-15 1,0-67 2395,-5 81-2187,26 9-223,-9 4-81,0 1 0,-1 1 0,0 1 0,0 0 0,0 1 0,-1 1 0,0 0 0,-1 1 0,0 1 0,12 13 0,-24-22-15,0-1 0,0 0 0,0 1-1,0 0 1,0-1 0,0 1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,-1 0-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 1 1,-1-1 0,-1 6 0,2-9 33,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 1,0 1-1,-4-31 181,4 23-199,1-1 1,0 0-1,1 1 1,0 0-1,0-1 1,0 1-1,1 0 1,0 0-1,1 0 1,7-11-1,54-69-581,-16 24-428,-44 56 856,0 0 0,-1 0 1,0 0-1,0-1 0,0 0 0,-1 0 1,0 0-1,-1 0 0,0 0 1,0-1-1,0 1 0,-1-1 1,-1 1-1,1-1 0,-1 1 0,-1-1 1,-1-11-1,-11 6 1224,12 14-1018,1 0 1,0 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 0 1,-1 0 0,1 1 0,0-1-1,-1 0 1,1 0 0,0 1-1,-1-1 1,1 0 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1-1,0 0 1,-1 1 0,1-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 0-1,0 1 1,-4 32 120,1-1 0,1 0 1,3 34-1,-1-57-338,1 0 1,0-1 0,0 1 0,0-1-1,1 0 1,1 1 0,-1-1-1,1 0 1,1 0 0,-1-1-1,1 1 1,0-1 0,1 1-1,0-1 1,0-1 0,0 1-1,7 5 1,4-4-3883,2-6-1991</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14164.96">13272 454 4466,'0'0'17758,"-3"4"-17590,-46 52 158,29-31-215,-2-1 0,-24 22 0,34-37 1366,34-11-1306,-8 3-171,0 1 0,-1 0 0,1 1 0,-1 1 0,0 0 0,24 11 1,38 11-5964,-50-22 320</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14513.63">13501 578 5346,'0'0'16968,"-8"-8"-15946,-25-20-440,32 27-577,1 1 0,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1-1,0-1 0,-1 1 1,1-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0-1 0,0 1 1,0-1-1,1 1 1,-4 28 103,3-29-109,0 6 1,0-1-1,1 1 1,0 0-1,0-1 1,1 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,1 0-1,4 4 1,4 6 5,2-1 0,22 19 0,11 14 8,-46-47 6,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 0-1,0 1 1,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,-35 4 327,29-3-329,-94 8-1689,99-26-5695,2-7 633</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15611.52">13552 398 11973,'0'0'10355,"5"-1"-9897,-3 1-429,0 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 1,-1 1-1,1-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 2-1,2 2 63,-1 1 0,1-1-1,-1 1 1,0-1 0,-1 1-1,3 8 1,4 15 409,8 56 0,-16-77-442,5 23 125,1 10 183,6 82 0,-13-122-363,0-1 1,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 1-1,0-1 1,0 0 0,1 0-1,-1 1 1,0-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,0 1 1,1-1 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1-1 1,0 1 0,0 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,1 0-1,-1 0 1,0-1-1,16-10 22,0-12 22,12-17 1,-26 39-66,-1-1 0,1 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,3-1 1,-3 3 15,1 0 1,0 0 0,-1 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,2 5 1,5 8 30,-1-3-1,1 0 0,0-1-1,1 0 1,0 0 0,14 11-1,-20-20-13,1 0-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0-1,0 0 1,0-1-1,0 1 1,1-1-1,-1 0 1,0 0 0,1-1-1,-1 1 1,1-1-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1-1 1,5-1-1,-4-1-1,1 1 0,-1-1 0,0 0-1,0 0 1,-1 0 0,1-1-1,-1 1 1,1-1 0,-1 0-1,0-1 1,0 1 0,-1-1 0,1 0-1,-1 0 1,4-7 0,-1 0 4,0 0 0,-1-1 1,0 0-1,-1 1 1,5-24-1,-4-53-27,-5 89 15,0-1-1,0 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 0,-1 0 1,1 1-1,-1-1 1,1 1-1,-1-1 0,1 0 1,-1 1-1,1-1 1,-1 1-1,0-1 0,1 1 1,-1 0-1,0-1 0,1 1 1,-1-1-1,0 1 1,1 0-1,-1 0 0,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,-1 1 1,1-2-3,-1 2-1,1-1 1,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,0 1-1,0-1 1,-1 1 0,1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,-1 0 1,2 0 0,-1 0 0,-2 3-1,-2 6-2,1 2-1,0-1 1,1 0 0,0 1-1,1-1 1,0 1-1,0 0 1,2 0 0,-1 0-1,3 21 1,-2-31 0,1 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-2 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1-1-1,0 1 1,-1 0-1,1-1 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,1 0 1,-1-1-1,0 1 1,0-1 0,5 0-1,-1 1-4,0-1-1,1 1 1,-1-1-1,0-1 0,0 1 1,0-1-1,0 0 1,0-1-1,9-3 1,-5 1-13,-1-2 1,1 0 0,-1 0 0,-1 0-1,1-1 1,-1-1 0,0 1 0,0-1-1,-1-1 1,0 0 0,-1 0 0,1 0-1,-2-1 1,1 1 0,-1-2 0,-1 1-1,0 0 1,0-1 0,-1 0 0,0 0-1,-1 0 1,0 0 0,-1 0 0,0-13-1,-1 23 22,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,-18 4 18,-12 15-30,25-10 21,0 1 0,1 0 0,1-1 0,0 2 0,0-1 0,1 0 0,0 1 0,0 0-1,2-1 1,-1 1 0,1 0 0,0 0 0,1 0 0,1 0 0,0 0 0,2 14 0,-2-23-11,-1 1-1,1-1 1,-1 0 0,1 1 0,0-1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1-1 0,0 1 0,0 0-1,1-1 1,-1 0 0,0 1 0,1-1 0,-1 0-1,0 0 1,0-1 0,1 1 0,-1 0 0,0-1-1,1 0 1,1 0 0,6-2-17,-1 0-1,0 0 1,0-1 0,0-1-1,0 1 1,-1-1 0,1-1-1,7-6 1,5-6-64,-1-1 0,-1-1 0,0-1-1,21-32 1,-30 37 44,0-1-1,-2 0 0,0 0 1,-1-1-1,0 0 1,-2 0-1,6-29 1,-1-30-167,-3 0 1,-4-129-1,-4 124 264,-3 87 759,-2 15-869,-2 43 146,4 1 1,6 127-1,0-144-45,0-12-89,3 0 0,14 59 0,-8-44-1018,-10-44-137</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15810.5">14312 353 9845,'0'0'17159,"103"-72"-16983,-6 37-64,1 3-31,-1-5-97,6 2 16,-25 6-161,-15 3 81,-34 8-576,-29 4-48,-5 5-1345,-43 9-8516</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:13:53.829"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">15 56 3858,'0'0'5738,"-1"-3"-4916,0 1-891,-8-21 2016,6 3-7936,3 12 2547</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:14:21.101"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">28 110 11685,'0'0'10253,"0"-6"-9397,0-16-45,0 16 1484,0 11-2220,0 258 444,0-149-4795,2-120-1302,3-1 3416,-2 3 82,7-13-6796</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="686.09">19 135 11045,'0'0'9714,"-4"-12"-9085,-9-34-223,13 43-382,-1 1 1,1 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,0 0 1,0 0-1,-1 0 0,2 0 1,-1 0-1,0 0 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,0-1-1,0 1 0,0 1 1,3-2-1,3-1 58,-1 0 1,0 1 0,1 0-1,0 0 1,-1 1 0,16-1-1,-22 2-76,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,1 39 89,-1-29-38,-1-1-38,1 0 0,-2-1 0,1 1-1,-2 0 1,1-1 0,-1 0-1,-1 1 1,0-1 0,0 0 0,-1-1-1,-1 1 1,1-1 0,-13 15 0,10-13-203,16-10-168,2-1 394,8 0-54,-6-1-80,1 1 1,-1 0 0,0 0 0,0 1-1,0 1 1,0 0 0,0 1-1,-1 0 1,21 9 0,-31-11 83,0-1 1,0 1 0,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-2 1-1,0 1 37,-1 0-1,1 0 0,0 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,-5 2 1,-6 2-16,0 0 0,0 0 0,-1-2 0,0 0 0,-1 0 0,1-2 0,-1 0 0,0 0 0,-23 0 0,40-17-12976,12 3 3912</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1149.86">313 169 11669,'0'0'7486,"-11"8"-6578,-32 29-79,40-34-744,1 0-1,0 1 0,0-1 1,0 0-1,0 1 1,0 0-1,1-1 0,-1 1 1,1 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,2 4-1,-2 10 72,1-16-145,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1-1 0,0 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,2 0 0,-1 0-3,0 0-1,0 1 1,-1-1 0,1 0-1,0-1 1,0 1 0,-1 0 0,1-1-1,0 0 1,-1 1 0,1-1 0,0 0-1,-1 0 1,1-1 0,-1 1 0,1 0-1,-1-1 1,0 0 0,0 1 0,0-1-1,3-3 1,-4 4-2,0 0 1,0-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1-1,0 0 0,0 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-3 0 1,-4-2-106,-1 1 0,0 0 1,0 1-1,0 0 0,0 0 1,-11 2-1,18-1-872,9 2-7258,13-1 6746,-18-2 145,23 1-3315</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1291.14">313 169 8084</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1492.24">326 169 8084,'121'18'3215,"-96"-14"4556,-30 24-5498,3-22-2110,1 1-1,0-1 1,0 1-1,1-1 1,-1 1 0,2 7-1,-1 7 229,30-22-188,-28 0-188,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-2-3 0,2 2 28,-1 1 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,-1 1-1,1 0 1,0 0 0,0 0 0,-5-2-1,-31-3-442,37 6-371,1 1 410,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,17 0-5199</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1785.44">579 54 7619,'0'0'11262,"-2"-7"-9803,-8-19-467,7 20-351,3 14 130,-1 67 180,3 89 445,-1-156-1358,0 0-1,1 0 0,0 0 1,0 0-1,1 0 0,6 13 1,-7-18-270,-1-1 0,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,3 1 1,-3-2-268,-1 0 1,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,2-1-1,6-6-6725</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2153.24">678 135 4978,'0'0'16368,"-2"-6"-15277,1 4-1028,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,-1 1 1,1 0 0,-1 0-1,-1-2 1,1 3-44,0 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 1 0,0-1-1,1 0 1,-1 0 0,0 1 0,1-1 0,-1 1-1,0-1 1,1 1 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,0 2 1,-7 3-10,1 1-1,0 1 0,0-1 1,1 2-1,0-1 0,1 1 1,-9 14-1,17-22-18,-1 0 0,0 1-1,1-1 1,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 0 0,0 1-1,3-1 1,5 3-16,0 1 4,0 2 0,0-1 0,0 1 0,-1 1-1,0-1 1,-1 2 0,14 12 0,-12-10-166,0 0 0,1-1 0,21 14 0,-27-18-1922</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:14:25.817"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 83 10997,'0'0'14938,"7"0"-14800,255 14 145,-166-12-240,-46 1 10,-1-3 1,94-11-1,-140 9-53,-3 2 168,-14-2-192,0 0 0,0 0 1,1-2-1,-1 1 0,1-2 0,-22-10 1,-9-2-38,-52-22 229,154 51-125,107 6 0,-153-17-54,-11-1 6,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,0 0 1,0-1-1,0 1 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 0,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,-1 1 1,-8 44 73,-1-26-33,-1-1 0,-1 0 0,-1-1 0,-27 31 0,6-7-102,17-23-467,-15 21-173,23-14-9004</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:14:27.622"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">54 102 7331,'0'1'16832,"-1"58"-16675,-1-19 55,2 1 0,12 77-1,-6-79 46,-1 0 0,-1 61 0,1-75-255,3-18-2286,3-13-3483,-1-11-993</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="408.18">39 127 11365,'0'0'10248,"-8"-12"-9819,-21-41-250,28 52-178,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,2-1 0,38-15-20,-34 14 14,3-1-3,0 1-1,0-1 1,0 2 0,0-1-1,0 1 1,1 1 0,-1 0-1,20 2 1,-28 0 5,0-1 1,0 0-1,0 1 0,0 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 1 0,0-1 1,-1 0-1,0 1 0,1 3 0,0 1 21,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,-1 8 0,0-10 54,-1 1-1,1-1 1,-1 0 0,-1 1-1,1-2 1,-1 1-1,1 0 1,-1-1-1,-1 1 1,1-1 0,-9 6-1,-61 36 472,60-37-555,7-6-355</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1931.67">448 245 10373,'0'0'10645,"-9"-6"-10133,0 1-325,-1 0 1,1 1-1,-1 0 0,0 0 1,-10-2-1,16 5-115,0 0-1,0 0 0,-1 0 1,1 1-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 1 0,0-1 1,0 1-1,0 0 1,-5 3-1,4-1-42,1-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,1 1 0,-1 0-1,1 0 1,-3 8 0,2-2-7,1 0 0,0 0 0,1 1 0,1 21 0,0-31-23,0 0 0,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,0-1 0,0 1 1,0 0-1,0-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,2 0 0,2 1-16,-1-1 0,1 0-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 0 0,-1-1-1,8-1 1,-10 2 7,-1-1 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1-1,-1-3 1,3-10 6,-2 0-1,0-29 0,-1 34 21,0 10 3,9 26-272,-6-22 249,0 0 1,1 0 0,-1 0 0,1 0 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1-1-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1-1 0,1 0 0,4 0 0,3 1-49,1-1 1,-1-1-1,0 0 1,0-1-1,19-5 0,-27 6 38,0 0 0,0-1 0,0 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1 0,1 1-1,-1-1 1,0 1 0,-1-1-1,1 0 1,0 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0-1-1,0 1 1,-2-7 0,1 10 34,1-1 0,-1 0 0,0 1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 1,-1-1-1,1 1 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 0,1 1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 1 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 1 1,-1 1-1,-1 12-18,1-1 0,0 1 1,1 0-1,0 0 0,2 0 0,-1 0 1,2-1-1,0 1 0,6 19 1,5 12 21,32 70 0,-30-84-14,-2 1 1,-1 1-1,-2 0 0,8 44 0,-17-69 5,6 68 50,-7-71-51,0 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,-1-1 0,0 1 0,0-1 0,-5 9 0,7-13 5,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,1-1 1,-1 1-1,0 0 0,1-1 0,-1 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,1 0 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,1 1 0,-1 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 0,-1-1 0,0-1 5,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-4 0,-3-12-100,1-1 0,1 0 0,1 0 0,1 0 0,0 0 0,2-1 0,0 1 0,1 0 0,1 0 0,1 1 0,0-1 0,1 1 0,15-33 0,-1 10-370,2 2-1,2 0 0,1 1 0,52-61 1,-71 94 467,-1 0 0,0-1 1,0 1-1,0-1 0,-1 0 1,0-1-1,0 1 0,-1 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,0 0 0,0 1 1,-1-1-1,1 0 0,-2-7 1,0 12 15,1 1 1,-1-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,-3 0 1,2 0-9,0 0 1,1-1-1,-1 1 1,0 0 0,0 1-1,0-1 1,1 0-1,-1 1 1,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,0 1-1,-3 2 1,1 4 2,0 1 0,1 0 0,0 0 1,1 0-1,-1 1 0,2-1 0,0 0 0,0 1 0,0-1 1,1 1-1,1-1 0,2 14 0,-3-19-23,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1-1 0,0 1 0,0 0 0,1-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1-1 0,1 1 0,-1 0 0,0-1 0,1 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0-1 0,6 1-1,-4 0-10,0-1 0,0 1 1,0-2-1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,4-8 0,2-3 13,-1 0 0,-1 0 0,-1 0 1,0-1-1,-1 0 0,-1 0 0,0 0 0,-1-1 0,-1 0 0,-1 1 0,-1-27 0,0 43 9,0 0 0,-1 0-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1 0,0-1-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,1 0-1,-1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0-1 0,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 1-1,-1 2-30,0 0 0,1 0-1,-1 1 1,1-1 0,1 1-1,-1-1 1,0 1-1,1-1 1,0 1 0,0 0-1,0-1 1,1 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,7 7-1,-2-5-32,0 1-1,0-1 0,1-1 0,0 0 0,0 0 1,0 0-1,1-1 0,-1 0 0,1-1 0,0 1 0,11 1 1,-13-4 11,26 10-96,-32-10 127,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 0 1,-1 0-1,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,-1 1 0,-5 5 39,1-1 1,-1 1-1,-1-1 0,1 0 0,-1 0 0,0-1 1,-13 8-1,-61 32-722,45-31-2914,1-5-5071</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:14:46.995"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 182 5090,'0'0'4610,"-5"-8"-4610</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="588.09">6 195 3009,'9'-9'10812,"-8"19"-263,-2 7-12704,-8 251 3185,9-267-1032,0 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,1-1-1,0 1 1,4-1-51,-1 0 1,1 0-1,-1 0 1,1-1-1,-1 0 1,9-4-1,-7 2 0,0 0 0,0-1-1,0 0 1,-1 0 0,0 0 0,0-1-1,-1 0 1,0 0 0,0-1 0,0 0-1,-1 1 1,1-1 0,-2-1 0,1 1-1,-1 0 1,0-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0-1,-1 0 1,-1-15 0,0 19 70,0 0 1,0 0 0,-1 0-1,0 0 1,1 0-1,-2 0 1,1 1-1,0-1 1,0 1 0,-1 0-1,0 0 1,0-1-1,0 2 1,0-1-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1 0-1,-8-3 1,1 1-12,1 0 0,-1 1 1,1 0-1,-1 1 0,0 0 0,0 0 0,-17 0 1,26 3-462,0 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,-1-1-1,1 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 0 1,2 3-1,6 5-6124</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1209.25">277 237 4946,'0'0'10442,"2"8"-9740,6 19 120,-2 1-1,0 0 1,1 34 0,-7-62-816,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,9-7 121,6-9-55,21-20-141,-35 34 58,1 1-1,-1-1 0,0 1 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1 0 1,0 1-1,-1-1 0,1 0 1,0 1-1,0 0 1,-1 0-1,1 0 0,4 0 1,-5 2 32,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 1-1,0-1 1,-1 0 0,0 1 0,1 0 0,-1-1 0,1 6 0,10 15 170,-10-21-180,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 0 0,1 0-1,-1 1 1,1-1 0,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0-1,4-1 1,-3 0-2,0-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,-1 1-1,1-6 1,1-30 35,-2 36-20,0 1-1,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,-2-1 0,2 2 600,-14 28-426,13-21-203,1-1 1,-1 1-1,1 0 1,1-1-1,-1 1 0,1 0 1,1 7-1,-1-13-104,0 1 0,0 0 0,0-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0 0,-1 0 0,3 1-1,22-1-3091,6 0-2250</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1597.31">837 156 11157,'0'0'7182,"-9"0"-6891,-31 2-139,39-2-145,0 1 0,0-1 0,0 0 0,0 1 0,1-1 1,-1 1-1,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0 32 5,1-25 2,-1-5-37,0-1 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 1,1 0-1,-1 0 0,0 0 0,1-1 1,-1 1-1,1 0 0,0-1 0,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,1 0 0,3 3 1,6 2-515,0-1 0,1 0 1,23 8-1,16 8-657,-52-22 1228,1 0 1,-1 0-1,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,1 0 0,-1 1 1,0-1-1,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 1 0,-1-1 0,-24 18 1867,20-15-1623,-19 11 454,15-9-746,-1 0 0,1 1 0,1 0 0,-1 1 1,-9 9-1,18-15-304,-3 1 7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1800.32">990 285 11205,'0'0'4850,"34"70"-4850,-19-56-16,-1-3-432,-4-8-2049,0-1-4226</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2044">1122 3 11493,'0'0'9349,"-5"-3"-9301,5 14-2706,0 9 481,0 5-2753</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2779">1276 262 10565,'0'0'10482,"-13"5"-9820,6-2-587,0-1-21,1 0 0,0 0 1,0 1-1,0 0 1,0 0-1,1 1 0,-1-1 1,1 1-1,0 0 1,0 1-1,0 0 0,1-1 1,-1 1-1,-4 9 1,5-6-45,0 0 1,1 0-1,1 0 0,-1 1 1,2 0-1,-1-1 1,1 1-1,0 0 1,1 0-1,0 10 0,0-19-31,0 1 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,0-1-1,1 1 1,0 0-71,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 0,0 0 1,-1 0-1,1 0 0,5-1 0,-3 0-83,0 1 0,0-2-1,0 1 1,1-1 0,-1 1-1,-1-1 1,1-1 0,0 1-1,8-6 1,-1-5-104,0 0 1,-1-1-1,-1 0 0,0 0 1,-1-1-1,0-1 0,-1 1 1,-1-2-1,-1 1 1,0-1-1,5-21 0,-5 7 323,5-53 0,-8-35 3695,-3 119-3214,0 8-293,-1 30-319,0-21 112,1 1 0,0-1 1,1 1-1,1-1 0,6 29 1,-6-42-37,-1 0 1,1 0-1,-1 0 1,1 0-1,1-1 1,-1 1-1,0 0 1,1-1-1,0 0 1,0 0-1,0 1 1,0-2-1,0 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,1 0-1,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 0-1,1-1 1,4 0-1,0 0-66,0 0-1,0-1 0,0 0 1,-1-1-1,1 0 1,0 0-1,-1-1 0,0 0 1,0 0-1,0-1 0,0 0 1,9-7-1,-14 9 107,1 0 0,0-1 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0-1,0 0 1,0 0 0,0 0 0,-1-1 0,0 1 0,1 0 0,-2-1-1,1 1 1,0-1 0,-1 1 0,0-1 0,0 1 0,-1-8 0,0 11-20,0-1 1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1-1,-3 1 1,0 0-25,-1-1-1,1 1 0,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,-7 5-1,7-1 3,-1 0 0,1 1 1,0-1-1,0 1 0,1 0 1,0 0-1,0 0 0,0 1 0,1-1 1,0 1-1,1-1 0,0 1 0,0-1 1,1 1-1,-1 0 0,2 0 0,0 9 1,0-14-10,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1-1-1,1 1 0,0 0 1,-1-1-1,1 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1-1-1,-1 1 0,0-1 1,0 1-1,4-1 1,8 2-569,1-1 0,0-1 0,17-1 1,-23 1-22,24-4-2950,-7-6-2669</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:15:03.944"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">441 997 1217,'0'0'7219,"-10"-3"-6571,9 2-633,-14-4 452,-1 1-1,1 0 1,-1 1-1,-28-2 1,42 5-168,1 0 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-2-3 1,-13-33 1992,11 19-1989,2-1 0,-2-25 1,5 38-34,-11-164 979,-12-118-703,-18 7-335,27 205 208,14 75-404,1 1 1,-1-1-1,0 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,1 0 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 0 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1 0-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,-21 3 76,-14 21-183,22-9 58,3-4 24,1 1 0,0 0 0,0 1 0,1-1 0,1 2-1,0-1 1,1 1 0,-9 25 0,9-12-123,17-49-105,11-26 249,4 0-1,-20 37-10,1 0-1,0 0 1,0 1 0,1-1-1,0 1 1,10-9 0,-16 18-12,1 0 1,-1 0 0,0 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1 1 0,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1 0 1,0 0-1,1-1 1,-1 1 0,2 2-1,42 36 23,-34-29-15,-4-3-30,1-1-1,0 0 1,1-1-1,-1 0 1,18 7 0,5 1-3385,-26-9 371</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:15:05.086"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">46 429 4834,'0'0'10880,"-2"-4"-9597,0 0-794,-4-16 2781,6 19-2755,0 1-477,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,-1 75 6,0-23 150,1 0 1,3 0-1,10 65 1,-12-113-757,1 15 1670,-1-12-3186</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="254.13">5 492 1825,'0'0'16695,"-1"-4"-16057,0 3-620,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,30-19 91,-28 19-106,2 0-52,4-4-46,0 1 0,0 1-1,1 0 1,-1 0-1,1 1 1,0 0-1,0 0 1,17-1 0,-26 5-85,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 1 0,1 2-983,0 11-3506</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="477.72">5 492 9124,'49'107'6195,"-30"-107"-5651,6-11 465,-1-4-625,5 4-128,-5-4-208,-4 4 16,-1 2-64,-9 6-208,0 3-816,-10 9-8725</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="676.71">90 747 112,'0'0'17400,"14"3"-17320,11-3 144,-1 0-224,5-11-624,0-4-1777,0-5-4002</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="913.58">357 507 11317,'0'0'10373,"-54"52"-9877,40-18-80,-1 1-96,1 0-239,9-6 31,-5-4-112,5-1-289,5-4-591,0-9-1313,0-2-1441</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1097.04">245 654 8404,'0'0'10116,"19"-9"-9507,-9 18 303,10 5-560,-6 4-272,6-4 0,-1 3-80,5-5-864,1-6-1041,-1-3-992,5-3-1617,-5 0-3234</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5055.93">731 577 6659,'0'0'12216,"-4"-6"-11471,1-2-575,-11-18 476,10 24-527,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0 0 0,0 0 0,0 1 0,-6 1 0,-7-1-8,12-1-103,1 1-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 1 1,0 0-1,0 1 0,0-1 1,0 1-1,1 0 0,-1 0 1,1 1-1,0-1 0,0 1 1,0 0-1,0 0 0,1 1 1,-1-1-1,1 1 1,0 0-1,1-1 0,-1 1 1,1 1-1,0-1 0,0 0 1,0 0-1,1 1 0,0-1 1,0 1-1,-1 10 0,2-13 0,0 1-1,0 0 0,0-1 0,0 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 0 1,0 1-1,1-1 0,3 5 1,-3-6 2,0 1 1,1-2-1,-1 1 1,1 0-1,-1 0 1,1-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 0-1,4 0 1,4 0-5,0 0 0,0-1 0,0 0 0,0-1-1,0-1 1,0 0 0,-1 0 0,1-1 0,-1-1 0,0 0 0,0 0 0,-1-1 0,1 0-1,-1 0 1,0-1 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,-1 0 0,1-1-1,8-16 1,-13 21-8,0 0-1,0-1 1,-1 1-1,1-1 1,-1 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,0 0 1,-1-9-1,0-13-18,1 28 19,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,-1 0-1,1 0 1,0-1 0,0 1-1,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1-1,0 0 1,-1 1 0,-15 15-66,14-11 68,-1-1 1,1 1-1,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 1 1,0-1-1,0 0 0,0 0 1,1 0-1,2 5 1,-2-6 3,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0-1-1,0 0 0,0 0 0,0 0 0,7-1 0,-5-1-6,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0-1-1,0 0 1,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,3-5 0,1-2-9,0 0 0,-1 0 1,0 0-1,-1-1 0,8-25 1,-10 25 0,-1 1 1,-1-1-1,0 1 1,-1-1-1,0 0 1,-1 1-1,-1-1 1,1 0 0,-2 1-1,0-1 1,0 1-1,-1-1 1,-1 1-1,0 0 1,0 0-1,-1 1 1,-1-1-1,0 1 1,0 0 0,-1 1-1,0-1 1,-1 2-1,-9-10 1,16 61 151,0-20-109,2 0-1,0 0 0,1 0 1,2-1-1,0 1 1,10 32-1,-10-46-88,-1 0 1,1 0-1,1 0 0,-1 0 0,1-1 1,0 1-1,1-1 0,0-1 0,0 1 1,0-1-1,1 0 0,0 0 0,0-1 1,0 0-1,1-1 0,-1 1 0,1-2 1,0 1-1,11 3 0,21 1-2803,-4-6-1969</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5842.13">1423 283 3858,'-1'2'20871,"-7"20"-20941,3 204 1010,5-180-853,0-40-81,0-1 0,1 1 0,0-1 0,0 0-1,0 0 1,0 1 0,1-1 0,0 0 0,0 0-1,3 5 1,-4-8-11,0 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 1,1-1-1,-1 1 0,0-1 1,0 1-1,0-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,3 0 0,-3-1-1,0-1 0,0 1 0,0 0-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1-3-1,14-40-48,-14 33 57,3-7-15,0 0 0,-2 0-1,2-32 1,-4 51 5,0 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 2 1,10 19 17,1 0 1,1-1 0,24 30 0,-34-46-14,0 0-1,0 0 1,0 0 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,1 0-1,-1 0 1,1 0 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,-1-1-1,1 1 1,5-2 0,-8 0 0,1 1 0,-1-1 0,0 0 1,0 0-1,1 0 0,-2 0 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,1-4 0,11-49 13,-10 32 6,-2-1 0,0 0 1,-1 1-1,-2-1 0,-4-28 0,3 39-16,0 0 0,0 0 1,-1 1-1,-1-1 0,0 1 0,-1 0 0,0 1 0,-1 0 1,-1 0-1,-9-13 0,-3 8-124,20 17 79,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 0,0 1 0,-2 42-5956,3-26 3336,-1 7-3386</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6585.77">1877 406 8548,'0'0'6835,"1"17"-5013,0-4-1566,-1-1 45,1 0 1,0-1-1,1 1 1,0 0-1,1 0 1,0-1-1,1 0 1,0 1-1,1-1 1,6 10 0,-9-17-195,1-1 0,-1 0 0,1 0 0,0 0 0,1 0 1,-1-1-1,0 1 0,1-1 0,-1 0 0,5 2 0,-7-3-76,0-1-1,-1 0 0,1 0 1,0 1-1,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,-1-1 0,1 1 1,1-1-1,-1 0-7,0 0 1,-1 0-1,1-1 1,0 1-1,-1 0 0,1 0 1,0 0-1,-1-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 0,0-1 1,0-1-1,0-20 82,0 13-65,1 0-1,-2-1 1,1 1 0,-1 0 0,-5-18 0,5 25-38,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 1 0,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 1-1,0-1 1,1 1-1,-1-1 1,0 1-1,0 0 0,0 0 1,-5-1-1,4 1-38,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,1 1 0,-1-1 0,-7 3 0,10-2-143,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1-1,0-1 1,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,0 0 0,0 0 0,0 2 0,0-3-42,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0-1,0-1 1,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,39-1-344,-30 1 309,35-2 721,-34 0 161,-1 2-1,1-1 1,0 2-1,0-1 1,14 4-1,-22-3-447,0 1 1,0-1-1,0 1 0,-1 0 1,1 0-1,0 0 0,-1 1 0,1-1 1,-1 1-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,0 1-1,1 0 0,2 6 0,-2-2 65,-1-1-1,1 0 0,-1 1 0,-1-1 0,1 1 1,-1 0-1,0-1 0,-1 1 0,0 11 0,0-19-25,-2-2-148,0-1 0,1 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,1 0-1,-1 1 1,1-5 0,2-49-686,-1 28 340,1-6-565,1 0-1,11-51 1,-7 51 489,-2 0 1,3-51-1,-8 59 724,0 20 4735,0 30-5064,-1 42 221,10 70 1,-7-115-348,2-1 0,0 1 0,1-1 1,2 1-1,-1-2 0,2 1 0,16 30 1,-22-47-162,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 0-1,1 0 1,0 0-1,4 3 1,23 1-5317,-11-6-1647</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6893.41">2399 332 8644,'0'0'9671,"-15"10"-9351,1-1-250,-11 6 43,1 2 0,-30 27-1,8-16-2,45-27-73,9-5 65,2 1-14,1 0 1,-1 0 0,1 2 0,0-1 0,-1 1-1,1 1 1,0 0 0,0 0 0,0 1 0,-1 1 0,1 0-1,0 0 1,-1 1 0,0 1 0,1 0 0,-1 0 0,-1 1-1,1 0 1,-1 1 0,0 0 0,0 0 0,0 1 0,-1 0-1,0 1 1,0 0 0,6 10 0,5-1-6767</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7432.57">2571 136 12214,'0'0'9489,"-2"13"-9195,0 20 67,0 0 1,2 1-1,5 36 1,3-8-135,-4-20-22,18 71 0,-18-117-194,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1-1 0,2-5 0,15-15 13,-16 20-37,0 0 0,0 1-1,0-1 1,0 1 0,0 1-1,1-1 1,0 1 0,0 0-1,0 0 1,0 1 0,0 0-1,0 0 1,1 0 0,-1 1-1,0 0 1,1 0 0,-1 1-1,1 0 1,0 0 0,6 1-1,-12 0 17,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,-1-1 0,1 1 0,-1-1 0,0 3 0,0 1 40,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 0 1,-1 1 0,1-1-1,-1 0 1,-3 4-1,-1-2-145,1 0 0,-1 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1-1,0-1 1,0 1 0,-1-1 0,1-1 0,-1 0 0,-11 2 0,20-5-39,0 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,1 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,0 0 1,1-3-1064,-1-21-4478</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8076.06">2823 364 11989,'0'0'9522,"4"9"-8449,-1 2-848,1 2 73,0-1 0,1 0-1,1 0 1,7 12 0,-12-20-267,1-1 1,0 0-1,1-1 0,-1 1 1,0 0-1,1-1 0,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,0-1 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1 0 0,0 0 1,1-1-1,4 1 0,-9-42 31,-1 39-60,0-1 1,0 1 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,0 1 0,1-1-1,-1 1 1,-4-2 0,-25-18 15,32 20-49,0 0 1,0 1-1,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,27-11-488,-25 11 485,15-7-213,18-6-77,2 1-1,-1 1 1,1 3-1,74-8 0,-107 41 1227,-6 22 498,0-39-1281,0 0 1,1 0 0,0 0 0,0-1 0,1 1 0,2 14-1,-2-21-114,-1 0 0,1 0 0,0 0 0,-1-1-1,1 1 1,0 0 0,0 0 0,0-1 0,-1 1 0,1-1-1,0 1 1,0 0 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,2-1 0,29-12 69,-29 9-64,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 0 0,1 1 1,-1-1-1,-1 0 0,1 0 1,1-9-1,-2 12-1,0 0 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 1 0,-1-1-1,1 1 1,-1 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0 0,0 1-1,1-1 1,-1 0 0,-3-1-1,-4-2-91,-1 0 0,0 1 0,0 0 0,0 1 1,-1 0-1,1 1 0,-1 0 0,1 1 0,-1 0 0,-11 1 0,21 1-124,1-1 1,-1 0-1,1 0 1,-1 1 0,1-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1 0 1,1-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 4-2727,0 4-6124</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8639.82">3439 22 5042,'0'0'18777,"0"-6"-18174,0-10-418,3 31-77,3 54 66,-4-40-12,8 74 162,7 132 540,-17-255-775,0-6-72,5-52 0,-3 68-33,0 0-1,1 0 0,0 0 1,0 1-1,1-1 0,1 1 0,-1 0 1,9-13-1,29-29-119,-40 48 98,1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 1,0 1-1,1-1 0,-1 0 1,1 1-1,-1 0 0,1 0 1,-1 0-1,7-1 0,-9 2-204,-6 29-300,-11 5 458,14-29 0,-1-1-1,1 1 1,0 0 0,0-1 0,1 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 9 0,3-12 69,-1 0 0,1-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,5 1-1,5 2-6,34 10 14,1-1-1,95 10 1,-38-18-6458,-85-4 1926</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11408.44">1215 1018 9092,'0'0'10029,"-3"-5"-8607,-7-9-225,6 20 185,5 37 490,0-15-2335,-2 15 502,1 0 0,3 0 0,1-1 0,18 80 0,-16-102-30,-4-10-9,1 1 0,1-1 0,-1 1 0,10 16 0,-11-25-6,0 1 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0-1 0,1 1 1,4 0-1,0 0-79,1-1 0,-1 0 1,0-1-1,0 0 1,1 0-1,-1-1 1,0 0-1,0-1 1,-1 1-1,1-2 0,0 1 1,-1-1-1,11-7 1,-9 4-578,0 0 0,0 0 1,-1 0-1,0-1 0,13-17 0,-19 22 111,0-1 0,0 1-1,-1-1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0-5 1,-1-10-4443</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11596.93">1333 1232 10981,'0'0'7235,"5"-6"-7219,14-2 32,5-4-48,5-2-112,-4-1-896,-6 4-721,1-4-1280,-11 1-2130</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11798.02">1260 994 11989,'0'0'9013,"-15"-17"-9237,49 17-737,10 0 209,14 0-1169,5 0-656,5 0-1825,-9 6-2161</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12197.09">1875 1023 13510,'0'0'7652,"-19"13"-7007,-60 44-245,66-45-303,0-1 0,1 1 0,0 1 0,1 1 0,0-1-1,1 2 1,-16 29 0,16-27-74,8-14-148,-32 66-260,29-40-4718,5-36-3443,0-16 7210,0 19 522,0-38 20,0-18 3134,0 19 9558,4 42-11791,-1 0 0,1 1-1,0 0 1,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,-1-1-1,0 1 1,4 5 0,5 7 110,28 39-200,-24-31 38,2-1-1,19 21 1,-32-39-566,0-1 1,1 1-1,0-1 1,0 0 0,0 0-1,0-1 1,1 0-1,-1 0 1,1 0 0,0 0-1,0-1 1,0 0-1,0 0 1,7 0-1,16-1-5542</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12931.29">2042 1099 9428,'0'0'10997,"-11"6"-10482,9-5-485,-2 0 21,0 1 0,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0 1 1,1-1 0,0 0-1,-1 1 1,1 0 0,0-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,0 7 1,-1 4 109,1 0 0,1 0 1,0 0-1,5 28 0,-5-40-146,1 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1 0,1-1-1,-1 0 1,0 1-1,0-1 1,1 0 0,-1 0-1,1-1 1,0 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,6 0 1,1 0-10,0 0 0,0-1 0,0-1 1,-1 0-1,1 0 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1-1 0,0 0 1,0 0-1,10-6 0,-14 6-13,0 1 1,0-1 0,0 0-1,-1 0 1,1-1-1,-1 1 1,0-1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-13 1,-1 11 7,0 1 0,-1-1 0,0 1 0,0-1 0,-2-9 0,2 16 7,1-1 1,-1 1 0,0-1-1,1 0 1,-1 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,-1 1 1,1-1 0,-1 0-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,0 0 1,1 0-1,-3 0 1,3 0-9,1 1 1,-1 0-1,0-1 1,0 1-1,1 0 0,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 2-1,-3 29-45,2-26 54,0 0-9,1 0 0,-1-1 0,1 1 1,0 0-1,1-1 0,-1 1 0,1 0 0,0-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 0 0,1 0 1,-1 0-1,4 5 0,-2-6-2,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 0 1,1 0-1,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0-1 1,0 0-1,8 0 0,-7-1-23,0 0-1,0-1 1,0 0 0,0 0-1,0 0 1,0-1-1,0 0 1,-1 0-1,0 0 1,1-1 0,-1 0-1,0 0 1,-1 0-1,1 0 1,-1-1 0,0 0-1,6-9 1,1-1-265,0-1 0,-1-1 0,-1 0 0,13-32 0,-12 19-238,-2 0-1,-1-1 0,-1 0 0,-2 0 0,-1 0 0,-1-57 0,-2 81 657,-1 0 1,0 0-1,-1 0 1,1 1-1,-1-1 0,-4-9 1,5 14-42,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,-1-1 0,1 0 0,-1 1 1,1-1-1,-1 1 0,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,0 1 0,1-1 0,-1 0 1,-3 0-1,4 2-71,0 0 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0-1,-1 0 1,1 0 0,0-1 0,1 4 0,-1-3-6,-2 18 111,1 1 1,1 0 0,4 34-1,-2-46-76,-1 0-1,2 0 1,-1 0 0,1-1-1,1 1 1,-1-1-1,1 0 1,1 0 0,-1 0-1,12 13 1,-1-3-36,1-1 0,1 0 0,0-1 0,22 14 0,-29-23-1012,0-1 0,1 0-1,0-1 1,0 0-1,21 6 1,2-4-5556</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13588.72">2984 813 9412,'0'0'9962,"-1"0"-9953,1 0-1,0-1 1,0 1 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 1-1,0-1 1,-1 0 0,1 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,0 0 1,1 1 0,-4 18 347,1 0 0,1 0 0,1 1 0,1-1 1,4 27-1,9 38 538,-13-78-849,1-1-1,-1 1 1,1 0-1,1-1 0,-1 1 1,1-1-1,-1 0 0,2 0 1,-1 0-1,0 0 1,8 7-1,-9-10-43,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 1,-1-1-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,4-2 0,-2 0-38,1 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1-1 0,5-6 0,-4-2 43,0-1 1,-1 1-1,0 0 1,-2-1-1,1 0 1,-2 1-1,1-1 1,-3-18-1,2 27 373,0 10-373,0 1 0,0-1 0,1 0 0,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 0,1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 1 1,0-2-1,1 1 0,0 0 0,-1-1 0,8 5 0,-4-4-13,0 0-1,0 0 1,1-1-1,0 0 1,-1 0-1,1-1 1,0 0 0,0 0-1,1-1 1,-1 0-1,0-1 1,16-1-1,-22 1 2,0 0-1,0-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1-1-1,0 1 0,1-1 1,1-3-1,0 1 9,-1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0-10 0,0-2 47,-1-1 0,-1 0 1,-4-32-1,3 41-42,-1 0-1,0 0 1,-1 1-1,0-1 1,-1 1-1,1 0 1,-1 0-1,-1 0 1,0 0-1,0 1 0,0 0 1,-1 0-1,0 0 1,0 1-1,0 0 1,-1 0-1,0 1 1,-8-6-1,14 11-37,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 2 0,0 6-1050,1 0 0,-1 0 0,1 0 0,2 15 0,0 0-2919,-2 5-3703</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14156.68">3565 968 10757,'0'0'8436,"-3"18"-7209,-1 7-917,1-8-102,1-1-1,0 1 0,1 26 0,1-42-195,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1-1 1,0 1 0,0 0-1,-1 0 1,1-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1 0,2 0-1,-1 0 13,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,3-1 0,0-5 83,0 0-1,0 0 1,-1 0 0,0 0 0,0 0 0,0-1 0,-1 0 0,0 1 0,0-1 0,-1 0 0,1-9 0,-2 13-49,1 0 0,-1-1 1,0 1-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 1 1,0-1-1,1 0 0,-2 1 0,1 0 1,0-1-1,-1 1 0,1 0 0,-1 0 1,-4-3-1,96 47-3523,-67-33 3500,-1 0-1,0 2 1,-1 0-1,0 2 1,-1 0-1,27 22 1,-45-33-31,0 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,-2 2-1,0-1 95,1 0-1,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,-1-1 1,1 1-1,0-1 1,-1 0-1,1 0 0,0 0 1,-1 0-1,-5-2 0,8 1-75,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-3 0,1-41-91,0 39 64,0-2-91,1 0 1,0 0-1,0 0 0,1 1 0,0-1 0,0 1 1,1 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,9-9-1,31-28-2320,1 11-3578,-29 23 906</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14437.96">3901 681 10853,'0'0'12288,"0"0"-12278,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 1-1,0 4 24,0-1 0,0 1 0,0 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,1 0-1,-1 0 1,2 7 0,16 57 368,-12-45-312,5 22-54,-8-29-249,0-1 0,1 1 0,1-1-1,1 0 1,0-1 0,15 28 0,2-20-4654,-2-19-3414,-6-4-1267</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14696.73">4109 867 12166,'0'0'8361,"-8"12"-8062,-72 102 247,164-108 684,47 32-8700,-103-34 1606</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16202.3">4382 866 10101,'0'0'11386,"-12"-3"-10954,-37-6-205,48 9-222,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 1,0-1-1,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 1 0,0 29 77,0-25-79,0-2 4,1 0 0,-1-1-1,1 1 1,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,1-1 0,-1 1-1,1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0-1,4 4 1,4 1-4,-1-1 1,1 0-1,0-1 0,13 6 0,14 7-43,-38-18 139,-42-1 608,41 0-702,0-1 0,0 1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 1,0-1-1,1-33-185,-1 25 67,2-4-111,0-1 0,1 0 1,1 1-1,0 0 1,1 0-1,1 0 0,11-21 1,8-24-643,-20 43 858,0 0 0,-1-1 0,-1 0-1,3-29 1,-5-4 3813,-2 69-3708,-2 7-72,1 1 0,0 0 1,2 0-1,1 0 0,1-1 1,2 1-1,0 0 0,2-1 1,14 42-1,-20-66-23,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 1,-1 0-1,1 1 0,1-1 0,0-1-3,1 0 1,0 0-1,-1-1 1,1 0-1,-1 1 1,0-1-1,0-1 1,0 1-1,4-3 1,-6 4-2,2-1-4,-1 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1-1,0 0 1,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,4 3 0,6 5 46,1 1 0,-1 1 1,12 16-1,-9-11 12,-13-14-41,0-1 0,0 1 0,1-1 1,-1 1-1,1-1 0,-1 0 0,1 0 0,0-1 0,0 1 1,-1 0-1,1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,7-1 0,-8-1-1,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 1,-1 1-1,0-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,-1 0 1,1-1-1,0 1 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,0-1 1,0 0-1,-1 1 0,2-5 1,2-7 6,0 1 0,-1-1 0,-1 0 0,0 1 0,-1-1 0,-1 0 0,-1-28 0,0 40-12,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,-3-3 0,4 3-7,0 1-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 1 0,-1-1-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0-1,0 1 1,-1-1 0,1 0-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 2 0,-5 15 11,1 1 1,1 0-1,0 0 1,-1 36 0,5-53-15,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,-1 0 1,1 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 1 1,0-2-1,1 1 1,1 0-1,49-3-5,-44 1-23,0-1 1,-1 0-1,1-1 0,-1 0 1,0 0-1,0 0 0,-1-1 0,1 0 1,-1-1-1,0 1 0,0-1 0,0 0 1,-1-1-1,0 1 0,0-1 0,-1 0 1,0 0-1,0-1 0,-1 0 1,1 1-1,-1-1 0,-1 0 0,0 0 1,0-1-1,1-15 0,-2 23 29,-1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0 0-1,1-1 1,-1 1 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,-3-1 1,0 1-5,0 0 0,0 0 1,0 0-1,0 0 0,-1 1 0,1 0 0,-7 0 0,0 0 17,10 1-12,0-1 1,-1 0 0,1 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,0 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 2 1,-12 36-34,12-33 46,0 0 0,0 1 0,1-1 0,0 0-1,0 0 1,1 0 0,-1 0 0,1 0 0,0 0 0,4 11 0,-4-14-8,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 1,1-1-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 1,1 0-1,-1 0 0,0 0 0,0 0 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1-1 0,5-2 0,3-2-8,0 0 0,-1-1 0,0-1 1,0 0-1,0 0 0,-1-1 0,0 0 0,8-12 0,-9 11-78,-1 0 0,-1-1 1,0-1-1,0 1 0,-1-1 1,0 0-1,-1 0 0,-1 0 1,0 0-1,3-24 0,-2-8-1194,-3-81-1,-3 60 433,2 47 674,-1 0 1,0 1-1,-5-20 1,4 28 734,0 1 0,-1 0 0,0 0 1,-7-14-1,10 22-533,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 0,-4 12-89,1 24 179,2 0 1,1 1-1,2-1 0,1 0 0,2 0 0,1-1 0,2 1 0,2-1 0,0-1 0,27 58 0,-28-73-489,19 38-2877,-27-56 2993,0 1-1,1-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,0-1 1,2 2-1,10-2-6532</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16415.83">5004 716 13558,'0'0'8468,"111"-67"-8452,-33 38-16,5-5-16,9 2-752,0 3-689,0 0-32,-9 6-159,-25 3-1954,-29 3-6771</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-12-21T17:15:43.368"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 11781,'0'0'10928,"0"4"-8110,9 31-2917,133 486 267,-97-348-136,-161-308 96,114 130-126,2 4 4,1 6-152,0-1 119,0 1 1,0 0 0,1-1 0,-1 0-1,1 1 1,0-1 0,0 0 0,0 0 0,1 0-1,0 0 1,-1 0 0,6 5 0,48 46 112,-45-46-107,2 4 20,-10-9-12,1 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,0-1 0,0 1 0,0-1 0,10 3 0,-14-6 15,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-3 0,2-3 11,9-24 79,14-55 0,-19 56-249,3 0-1,12-29 1,-22 58-72,1-1 0,0 1 1,-1-1-1,1 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,1 0-1,-1 0 0,0 1 1,1-1-1,1-1 0,17 0-10440</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1030.86">346 1188 7619,'0'0'8084,"0"-37"-4082,0 35-3936,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 0,-2 1 0,2-1-64,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 1,1 1-1,-1 0 0,0 0 0,0 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 1 0,0-1 0,0 0 1,-1 4-1,1-1-30,0 0-1,1-1 1,-1 1 0,1 0 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0-1,1-1 1,0 1 0,1 0 0,-1-1-1,1 0 1,0 1 0,0-1 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0-1-1,0 1 1,8 5 0,16 14-494,-2-2-431,-1 1 1,0 1-1,23 31 0,-46-53 979,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 1,1 0-1,-1 0 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 0 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,-1 0-1,-58 7 1380,47-6-1314,-104 2 400,116-3-1758</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2957.48">479 1407 9236,'0'0'7228,"10"-14"-6831,2-2-316,0 1 61,0-1 1,0 0-1,-2-1 0,15-30 0,-22 40-126,-1-1 0,0 1 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-2 1 0,1-1 0,-1 0 0,-2-7 0,2 10 39,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 1-1,-1 0 1,1 0 0,-1 0 0,0 0 0,-1 1 0,1-1 0,-9-4 0,13 8-37,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,0 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,0 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0 0-1,0 21-104,0-19 162,-1 37 41,0-6 33,2 0 0,5 35 0,-4-58-105,0-1 1,0 0-1,1 0 0,1 0 0,-1 0 1,1 0-1,1-1 0,0 1 0,0-1 0,1-1 1,7 9-1,-12-16-22,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 0-1,0 1 1,0-1 0,0 0-1,1-1 1,41-43 38,-26 27-26,-17 18-40,1-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 1 1,-1 0-1,1-1 0,0 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0 1-1,26 41 111,-14-21-48,-10-18-47,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,1 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,0 0 0,0 0 1,0-1-1,0 1 0,1-1 0,-1 0 0,0 0 1,1 0-1,7 0 0,-8-2-3,-1 1 0,1-1 0,-1 0 0,1 0-1,-1-1 1,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0-1-1,0 1 1,0 0 0,-1 0 0,1-1 0,0-5 0,3-4-32,-1 0 1,-1-1-1,0 0 0,-1 0 0,0 0 1,-1 0-1,0 0 0,-1 0 1,-3-15-1,3 27 14,-1 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1 0 0,0-1-1,1 1 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,-2 0 1,-1 39-95,4-29 100,1-1 0,1 1-1,0 0 1,0-1 0,0 1 0,1 0-1,3 8 1,-4-14 5,0-1 0,1 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,5 0 0,-5 0 4,0 1 0,0-1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 1,1 0-1,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-7 0,1-2-30,-1-1 1,0 0-1,0 0 0,-1 1 0,-1-19 0,-3 30 0,0 0-1,1 1 1,-1-1-1,0 1 1,1 0-1,-1-1 1,0 1 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,1 0 1,-1-1 0,0 1-1,-4 3 1,4 7 19,1 0 1,1 1 0,-1-1-1,2 1 1,-1 0 0,2-1-1,-1 1 1,4 15 0,-3-23 10,-1-1 1,1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,0-1 0,0 1 0,0-1-1,0 1 1,1-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0-1-1,-1 1 1,1-1 0,0 0 0,0 0-1,1 0 1,-1 0 0,4 0-1,-3 0 5,0 0 0,0-1 0,1 0-1,-1 1 1,0-2 0,0 1 0,1 0-1,-1-1 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,0 0 1,-1-1 0,1 1 0,-1-1-1,5-4 1,3-5-52,0-1 1,-1-1-1,0 0 0,-2 0 1,1-1-1,-2 0 0,0 0 0,-1-1 1,0 0-1,-1 0 0,-1-1 0,0 1 1,-2-1-1,1 0 0,-2 0 0,-1-30 1,1 9-183,0 22 210,0 1 0,-1-1 0,-4-25-1,4 40 52,0 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1-1-1,-1 1 1,2 0-29,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,-3 70 33,1-37 90,1 1 1,6 64-1,-4-91-108,0 0 0,1 1-1,0-1 1,0 0 0,1-1-1,0 1 1,0 0 0,1-1-1,0 0 1,0 1 0,1-2-1,0 1 1,0 0-1,0-1 1,1 0 0,0-1-1,7 7 1,-11-11-12,-1 0 1,0 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1-1-1,1 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,0 0 1,0 0-1,-1 1 0,1-1 1,0-1-1,0 1 1,-1 0-1,1 0 0,0-1 1,0 1-1,-1-1 1,1 1-1,3-2 0,-2-1 1,0 1 0,-1 0-1,1-1 1,-1 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,1-3 0,2-9 27,0-1 1,-1 1-1,-1-1 1,2-24 0,-4 30-8,2-48-10,-3 56-17,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 1 1,-2-5-1,4 6-15,0 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1 0,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,-5 17-129,3 19 155,2-27-12,1-1-1,0 1 1,0 0 0,1-1-1,0 1 1,0-1-1,1 1 1,0-1 0,0 0-1,1 0 1,0 0-1,0-1 1,1 1 0,0-1-1,1 0 1,11 12-1,-10-12 7,0 0-1,-1 0 0,-1 1 0,1 0 0,8 16 1,-13-21-9,0-1 0,-1 0 0,1 0 0,0 0 1,-1 1-1,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,-1-1 0,-2 3 0,-5 4-265,0 0 0,-1-1 0,-19 12 0,24-16-654,-1-1-1,1 0 1,-1 0 0,0 0 0,-11 1 0,-4-2-5109</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3151.7">1180 1174 7523,'0'0'13783,"153"-61"-13751,-104 50-32,-5-1-1489,-9 7-2161,-11-1-5314</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3041,34 +5111,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A52A56-0CEC-4448-A2E0-2F135D4045E0}">
-  <dimension ref="B2:D283"/>
+  <dimension ref="B2:J296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H297" sqref="H297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="1.73046875" customWidth="1"/>
     <col min="2" max="2" width="43.46484375" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3079,1003 +5150,1063 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:4" ht="17.649999999999999">
+      <c r="B9" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4">
       <c r="B12" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4">
       <c r="B13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="2:4" ht="17.649999999999999">
+      <c r="B15" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2">
       <c r="B18" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2">
       <c r="B19" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2">
       <c r="B20" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:2" ht="17.649999999999999">
+      <c r="B22" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="2:2">
       <c r="B24" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2">
       <c r="B25" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2">
       <c r="B26" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2">
       <c r="B27" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B31" s="6" t="s">
+    <row r="31" spans="2:2" ht="17.649999999999999">
+      <c r="B31" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B35" s="8" t="s">
+    <row r="35" spans="2:2" ht="15.75">
+      <c r="B35" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2">
       <c r="B37" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2">
       <c r="B38" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2">
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2">
       <c r="B40" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B42" s="8" t="s">
+    <row r="42" spans="2:2" ht="15.75">
+      <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B43" s="7"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2">
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="2:2">
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2">
       <c r="B45" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2">
       <c r="B46" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:2">
       <c r="B47" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B49" s="8" t="s">
+    <row r="49" spans="2:2" ht="15.75">
+      <c r="B49" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2">
+      <c r="B50" s="4"/>
+    </row>
+    <row r="51" spans="2:2">
       <c r="B51" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2">
       <c r="B52" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:2">
       <c r="B53" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:2">
       <c r="B54" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B56" s="8" t="s">
+    <row r="56" spans="2:2" ht="15.75">
+      <c r="B56" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:2">
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="2:2">
       <c r="B58" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:2">
       <c r="B59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:2">
       <c r="B60" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:2">
       <c r="B61" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B63" s="8" t="s">
+    <row r="63" spans="2:2" ht="15.75">
+      <c r="B63" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B64" s="7"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:2">
+      <c r="B64" s="4"/>
+    </row>
+    <row r="65" spans="2:2">
       <c r="B65" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2">
       <c r="B66" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2">
       <c r="B67" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:2">
       <c r="B68" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B70" s="8" t="s">
+    <row r="70" spans="2:2" ht="15.75">
+      <c r="B70" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B71" s="7"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:2">
+      <c r="B71" s="4"/>
+    </row>
+    <row r="72" spans="2:2">
       <c r="B72" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:2">
       <c r="B73" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:2">
       <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:2">
       <c r="B75" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B77" s="8" t="s">
+    <row r="77" spans="2:2" ht="15.75">
+      <c r="B77" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B78" s="7"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:2">
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="2:2">
       <c r="B79" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:2">
       <c r="B80" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:2">
       <c r="B81" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:2">
       <c r="B82" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B85" s="6" t="s">
+    <row r="85" spans="2:2" ht="17.649999999999999">
+      <c r="B85" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:2">
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="2:2">
       <c r="B87" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:2">
       <c r="B88" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:2">
       <c r="B89" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:2">
       <c r="B90" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:2">
       <c r="B91" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:2">
       <c r="B92" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:2">
       <c r="B93" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:2">
       <c r="B95" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B97" s="6" t="s">
+    <row r="97" spans="2:2" ht="17.649999999999999">
+      <c r="B97" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B98" s="7"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2">
+      <c r="B98" s="4"/>
+    </row>
+    <row r="99" spans="2:2">
       <c r="B99" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:2">
       <c r="B100" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:2">
       <c r="B101" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:2">
       <c r="B102" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B104" s="6" t="s">
+    <row r="104" spans="2:2" ht="17.649999999999999">
+      <c r="B104" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B105" s="7"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:2">
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="2:2">
       <c r="B106" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:2">
       <c r="B107" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:2">
       <c r="B108" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:2">
       <c r="B109" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B111" s="6" t="s">
+    <row r="111" spans="2:2" ht="17.649999999999999">
+      <c r="B111" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B112" s="7"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:2">
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="2:2">
       <c r="B113" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:2">
       <c r="B114" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:2">
       <c r="B115" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:2">
       <c r="B116" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B118" s="6" t="s">
+    <row r="118" spans="2:2" ht="17.649999999999999">
+      <c r="B118" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B119" s="7"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:2">
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="2:2">
       <c r="B120" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:2">
       <c r="B121" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:2">
       <c r="B122" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:2">
       <c r="B123" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B127" s="6" t="s">
+    <row r="127" spans="2:2" ht="17.649999999999999">
+      <c r="B127" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B128" s="7"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:2">
+      <c r="B128" s="4"/>
+    </row>
+    <row r="129" spans="2:2">
       <c r="B129" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B130" s="7"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:2">
+      <c r="B130" s="4"/>
+    </row>
+    <row r="131" spans="2:2">
       <c r="B131" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B132" s="7"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:2">
+      <c r="B132" s="4"/>
+    </row>
+    <row r="133" spans="2:2">
       <c r="B133" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B134" s="7"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:2">
+      <c r="B134" s="4"/>
+    </row>
+    <row r="135" spans="2:2">
       <c r="B135" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B139" s="6" t="s">
+    <row r="139" spans="2:2" ht="17.649999999999999">
+      <c r="B139" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:2">
       <c r="B141" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B142" s="7"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:2">
+      <c r="B142" s="4"/>
+    </row>
+    <row r="143" spans="2:2">
       <c r="B143" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:2">
       <c r="B144" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:2">
       <c r="B145" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:2">
       <c r="B146" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B158" s="9" t="s">
+    <row r="158" spans="2:2">
+      <c r="B158" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B160" s="6" t="s">
+    <row r="160" spans="2:2" ht="17.649999999999999">
+      <c r="B160" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B161" s="7"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:2">
+      <c r="B161" s="4"/>
+    </row>
+    <row r="162" spans="2:2">
       <c r="B162" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:2">
       <c r="B163" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B165" s="6" t="s">
+    <row r="165" spans="2:2" ht="17.649999999999999">
+      <c r="B165" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B166" s="7"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:2">
+      <c r="B166" s="4"/>
+    </row>
+    <row r="167" spans="2:2">
       <c r="B167" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B168" s="7"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:2">
+      <c r="B168" s="4"/>
+    </row>
+    <row r="169" spans="2:2">
       <c r="B169" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B170" s="7"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:2">
+      <c r="B170" s="4"/>
+    </row>
+    <row r="171" spans="2:2">
       <c r="B171" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B172" s="7"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:2">
+      <c r="B172" s="4"/>
+    </row>
+    <row r="173" spans="2:2">
       <c r="B173" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B175" s="6" t="s">
+    <row r="175" spans="2:2" ht="17.649999999999999">
+      <c r="B175" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B176" s="7"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:2">
+      <c r="B176" s="4"/>
+    </row>
+    <row r="177" spans="2:2">
       <c r="B177" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="B179" s="6" t="s">
+    <row r="179" spans="2:2" ht="17.649999999999999">
+      <c r="B179" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B181" s="9" t="s">
+    <row r="181" spans="2:2">
+      <c r="B181" s="6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B183" s="9" t="s">
+    <row r="183" spans="2:2">
+      <c r="B183" s="6" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B184" s="7"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:2">
+      <c r="B184" s="4"/>
+    </row>
+    <row r="185" spans="2:2">
       <c r="B185" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:2">
       <c r="B186" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:2">
       <c r="B187" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B189" s="9" t="s">
+    <row r="189" spans="2:2">
+      <c r="B189" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B190" s="7"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:2">
+      <c r="B190" s="4"/>
+    </row>
+    <row r="191" spans="2:2">
       <c r="B191" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:2">
       <c r="B192" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:2">
       <c r="B193" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B195" s="9" t="s">
+    <row r="195" spans="2:2">
+      <c r="B195" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B196" s="7"/>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:2">
+      <c r="B196" s="4"/>
+    </row>
+    <row r="197" spans="2:2">
       <c r="B197" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:2">
       <c r="B198" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:2">
       <c r="B199" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B201" s="9" t="s">
+    <row r="201" spans="2:2">
+      <c r="B201" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B202" s="7"/>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:2">
+      <c r="B202" s="4"/>
+    </row>
+    <row r="203" spans="2:2">
       <c r="B203" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:2">
       <c r="B204" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:2">
       <c r="B205" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B207" s="9" t="s">
+    <row r="207" spans="2:2">
+      <c r="B207" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B208" s="7"/>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:2">
+      <c r="B208" s="4"/>
+    </row>
+    <row r="209" spans="2:2">
       <c r="B209" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:2">
       <c r="B210" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:2">
       <c r="B211" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B213" s="9" t="s">
+    <row r="213" spans="2:2">
+      <c r="B213" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B214" s="7"/>
-    </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:2">
+      <c r="B214" s="4"/>
+    </row>
+    <row r="215" spans="2:2">
       <c r="B215" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="216" spans="2:2">
       <c r="B216" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="217" spans="2:2">
       <c r="B217" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B219" s="9" t="s">
+    <row r="219" spans="2:2">
+      <c r="B219" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B220" s="7"/>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="2:2">
+      <c r="B220" s="4"/>
+    </row>
+    <row r="221" spans="2:2">
       <c r="B221" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="2:2">
       <c r="B222" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:2">
       <c r="B223" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B225" s="9" t="s">
+    <row r="225" spans="2:2">
+      <c r="B225" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B226" s="7"/>
-    </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="226" spans="2:2">
+      <c r="B226" s="4"/>
+    </row>
+    <row r="227" spans="2:2">
       <c r="B227" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="228" spans="2:2">
       <c r="B228" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="229" spans="2:2">
       <c r="B229" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B231" s="9" t="s">
+    <row r="231" spans="2:2">
+      <c r="B231" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B232" s="7"/>
-    </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="232" spans="2:2">
+      <c r="B232" s="4"/>
+    </row>
+    <row r="233" spans="2:2">
       <c r="B233" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="234" spans="2:2">
       <c r="B234" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="235" spans="2:2">
       <c r="B235" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B237" s="9" t="s">
+    <row r="237" spans="2:2">
+      <c r="B237" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B238" s="7"/>
-    </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:2">
+      <c r="B238" s="4"/>
+    </row>
+    <row r="239" spans="2:2">
       <c r="B239" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:2">
       <c r="B240" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:2">
       <c r="B241" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B243" s="9" t="s">
+    <row r="243" spans="2:2">
+      <c r="B243" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B244" s="7"/>
-    </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:2">
+      <c r="B244" s="4"/>
+    </row>
+    <row r="245" spans="2:2">
       <c r="B245" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:2">
       <c r="B246" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="247" spans="2:2">
       <c r="B247" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B249" s="9" t="s">
+    <row r="249" spans="2:2">
+      <c r="B249" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B250" s="7"/>
-    </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="2:2">
+      <c r="B250" s="4"/>
+    </row>
+    <row r="251" spans="2:2">
       <c r="B251" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:2">
       <c r="B252" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="253" spans="2:2">
       <c r="B253" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B255" s="9" t="s">
+    <row r="255" spans="2:2">
+      <c r="B255" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B256" s="7"/>
-    </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="256" spans="2:2">
+      <c r="B256" s="4"/>
+    </row>
+    <row r="257" spans="2:2">
       <c r="B257" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="258" spans="2:2">
       <c r="B258" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="259" spans="2:2">
       <c r="B259" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B261" s="9" t="s">
+    <row r="261" spans="2:2">
+      <c r="B261" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B262" s="7"/>
-    </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="262" spans="2:2">
+      <c r="B262" s="4"/>
+    </row>
+    <row r="263" spans="2:2">
       <c r="B263" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="264" spans="2:2">
       <c r="B264" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="265" spans="2:2">
       <c r="B265" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B267" s="9" t="s">
+    <row r="267" spans="2:2">
+      <c r="B267" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B268" s="7"/>
-    </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="268" spans="2:2">
+      <c r="B268" s="4"/>
+    </row>
+    <row r="269" spans="2:2">
       <c r="B269" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="270" spans="2:2">
       <c r="B270" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="271" spans="2:2">
       <c r="B271" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B273" s="9" t="s">
+    <row r="273" spans="2:3">
+      <c r="B273" s="6" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B274" s="7"/>
-    </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="274" spans="2:3">
+      <c r="B274" s="4"/>
+    </row>
+    <row r="275" spans="2:3">
       <c r="B275" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="276" spans="2:3">
       <c r="B276" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="277" spans="2:3">
       <c r="B277" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B279" s="9" t="s">
+    <row r="279" spans="2:3">
+      <c r="B279" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B280" s="7"/>
-    </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="280" spans="2:3">
+      <c r="B280" s="4"/>
+    </row>
+    <row r="281" spans="2:3">
       <c r="B281" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="282" spans="2:3">
       <c r="B282" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="283" spans="2:3">
       <c r="B283" s="2" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="287" spans="2:3">
+      <c r="C287" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="288" spans="2:3">
+      <c r="C288" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="289" spans="3:10">
+      <c r="C289" t="s">
+        <v>74</v>
+      </c>
+      <c r="E289" t="s">
+        <v>271</v>
+      </c>
+      <c r="G289" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="290" spans="3:10">
+      <c r="C290" t="s">
+        <v>270</v>
+      </c>
+      <c r="J290" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="291" spans="3:10">
+      <c r="C291" t="s">
+        <v>99</v>
+      </c>
+      <c r="J291" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="292" spans="3:10">
+      <c r="C292" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="293" spans="3:10">
+      <c r="C293" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="294" spans="3:10">
+      <c r="C294" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="296" spans="3:10">
+      <c r="E296" t="s">
+        <v>276</v>
+      </c>
+      <c r="F296" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4088,11 +6219,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C134CB0D-5D7A-4940-AF7C-5BEA146026FB}">
   <dimension ref="B2:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35:O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.9296875" customWidth="1"/>
@@ -4111,43 +6242,43 @@
     <col min="19" max="19" width="15.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13">
       <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:13">
       <c r="B5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13">
       <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" s="1" customFormat="1"/>
+    <row r="12" spans="2:13">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -4158,7 +6289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:13">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -4172,7 +6303,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:13">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -4201,7 +6332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:13">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -4221,7 +6352,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:12">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -4235,7 +6366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:12">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -4249,7 +6380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:12">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -4260,7 +6391,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:12">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -4271,17 +6402,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:12" s="1" customFormat="1">
       <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:12" s="1" customFormat="1">
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:12">
       <c r="H27" t="s">
         <v>46</v>
       </c>
@@ -4295,7 +6426,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:12">
       <c r="I28" t="s">
         <v>48</v>
       </c>
@@ -4306,7 +6437,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:12">
       <c r="I29" t="s">
         <v>50</v>
       </c>
@@ -4317,7 +6448,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:12">
       <c r="I30" t="s">
         <v>52</v>
       </c>
@@ -4328,28 +6459,28 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:20" s="1" customFormat="1">
       <c r="B33" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:20">
       <c r="B35" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
       <c r="O35" t="s">
         <v>62</v>
       </c>
@@ -4363,204 +6494,204 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+    <row r="36" spans="2:20">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
       <c r="O36" t="s">
         <v>66</v>
       </c>
       <c r="P36" t="s">
         <v>67</v>
       </c>
-      <c r="S36" s="5" t="s">
+      <c r="S36" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="T36" s="5" t="s">
+      <c r="T36" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:20">
       <c r="B37" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
       <c r="O37" t="s">
         <v>68</v>
       </c>
       <c r="P37" t="s">
         <v>70</v>
       </c>
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+    </row>
+    <row r="38" spans="2:20">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
       <c r="O38" t="s">
         <v>69</v>
       </c>
       <c r="P38" t="s">
         <v>71</v>
       </c>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+    </row>
+    <row r="39" spans="2:20">
       <c r="B39" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
       <c r="O39" t="s">
         <v>73</v>
       </c>
       <c r="P39" t="s">
         <v>72</v>
       </c>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+    </row>
+    <row r="40" spans="2:20">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
       <c r="O40" t="s">
         <v>75</v>
       </c>
       <c r="P40" t="s">
         <v>76</v>
       </c>
-      <c r="R40" s="5" t="s">
+      <c r="R40" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+    </row>
+    <row r="41" spans="2:20">
       <c r="B41" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
       <c r="O41" t="s">
         <v>78</v>
       </c>
       <c r="P41" t="s">
         <v>79</v>
       </c>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+    </row>
+    <row r="42" spans="2:20">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
       <c r="O42" t="s">
         <v>83</v>
       </c>
       <c r="P42" t="s">
         <v>80</v>
       </c>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+    </row>
+    <row r="43" spans="2:20">
       <c r="O43" t="s">
         <v>81</v>
       </c>
       <c r="P43" t="s">
         <v>81</v>
       </c>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+    </row>
+    <row r="44" spans="2:20">
       <c r="O44" t="s">
         <v>88</v>
       </c>
       <c r="P44" t="s">
         <v>92</v>
       </c>
-      <c r="R44" s="5" t="s">
+      <c r="R44" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="T44" s="5"/>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="T44" s="8"/>
+    </row>
+    <row r="45" spans="2:20">
       <c r="M45" t="s">
         <v>90</v>
       </c>
@@ -4573,10 +6704,10 @@
       <c r="P45" t="s">
         <v>93</v>
       </c>
-      <c r="R45" s="5"/>
-      <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R45" s="8"/>
+      <c r="T45" s="8"/>
+    </row>
+    <row r="46" spans="2:20">
       <c r="L46" t="s">
         <v>91</v>
       </c>
@@ -4589,10 +6720,10 @@
       <c r="O46" t="s">
         <v>85</v>
       </c>
-      <c r="R46" s="5"/>
-      <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R46" s="8"/>
+      <c r="T46" s="8"/>
+    </row>
+    <row r="47" spans="2:20">
       <c r="M47" t="s">
         <v>90</v>
       </c>
@@ -4605,10 +6736,10 @@
       <c r="P47" t="s">
         <v>95</v>
       </c>
-      <c r="R47" s="5"/>
-      <c r="T47" s="5"/>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="R47" s="8"/>
+      <c r="T47" s="8"/>
+    </row>
+    <row r="48" spans="2:20">
       <c r="M48" t="s">
         <v>90</v>
       </c>
@@ -4621,10 +6752,10 @@
       <c r="P48" t="s">
         <v>96</v>
       </c>
-      <c r="R48" s="5"/>
-      <c r="T48" s="5"/>
-    </row>
-    <row r="49" spans="15:20" x14ac:dyDescent="0.45">
+      <c r="R48" s="8"/>
+      <c r="T48" s="8"/>
+    </row>
+    <row r="49" spans="15:20">
       <c r="O49" t="s">
         <v>98</v>
       </c>
@@ -4637,7 +6768,7 @@
       <c r="S49" t="s">
         <v>100</v>
       </c>
-      <c r="T49" s="5"/>
+      <c r="T49" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4654,4 +6785,472 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC1880C-FC03-4559-9958-D373C8DDE1FE}">
+  <dimension ref="B2:M135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="3.06640625" customWidth="1"/>
+    <col min="2" max="2" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" customWidth="1"/>
+    <col min="4" max="4" width="29.46484375" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="I2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
+        <v>285</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" t="s">
+        <v>287</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="12" customFormat="1"/>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="D18" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="D19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="17.649999999999999">
+      <c r="B23" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="17.649999999999999">
+      <c r="B32" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="17.649999999999999">
+      <c r="B41" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="17.649999999999999">
+      <c r="B52" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" s="12" customFormat="1"/>
+    <row r="61" spans="2:4">
+      <c r="B61" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="C62" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="67" spans="3:13">
+      <c r="C67" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="76" spans="3:13">
+      <c r="C76" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" spans="3:13">
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+    </row>
+    <row r="80" spans="3:13">
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+    </row>
+    <row r="81" spans="3:13">
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+    </row>
+    <row r="82" spans="3:13">
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+    </row>
+    <row r="84" spans="3:13">
+      <c r="C84" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="89" spans="3:13">
+      <c r="C89" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="93" spans="3:13">
+      <c r="C93" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="C99" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="C100">
+        <f>5+6</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" t="s">
+        <v>353</v>
+      </c>
+      <c r="C102" t="s">
+        <v>349</v>
+      </c>
+      <c r="D102" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" t="s">
+        <v>354</v>
+      </c>
+      <c r="C108" t="s">
+        <v>351</v>
+      </c>
+      <c r="D108" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="C111" t="s">
+        <v>355</v>
+      </c>
+      <c r="D111" s="12"/>
+    </row>
+    <row r="113" spans="3:4">
+      <c r="C113" t="s">
+        <v>356</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4">
+      <c r="C115" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4">
+      <c r="C120" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4">
+      <c r="C124" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3">
+      <c r="C129" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3">
+      <c r="C134" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3">
+      <c r="C135" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H79:M82"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>